<commit_message>
Updating to include 2024 Data
</commit_message>
<xml_diff>
--- a/Election Math/election_margin_mix_v3.xlsx
+++ b/Election Math/election_margin_mix_v3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://penno365-my.sharepoint.com/personal/dmoratz_upenn_edu/Documents/Documents/Classes/Research/Election Math/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\My PC (LAPTOP-IKUHQKMA)\Documents\GitHub\election_math\Election Math\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="8_{69BC1A8B-9681-4F8C-80CA-B5D0D453FF23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5ED74077-647B-45A7-88C3-DF5F48673B6E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66593D4C-C19C-4906-A8B4-625B91BE0EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="867" activeTab="7" xr2:uid="{88BD8E8E-6581-40F7-95E1-0D4A8455A63F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="867" activeTab="8" xr2:uid="{88BD8E8E-6581-40F7-95E1-0D4A8455A63F}"/>
   </bookViews>
   <sheets>
     <sheet name="Grimmer Black Vote check" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,6 @@
     <sheet name="Pizza Example" sheetId="16" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -871,10 +870,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -16276,6 +16271,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="J29:P29"/>
+    <mergeCell ref="R29:W29"/>
+    <mergeCell ref="J38:P38"/>
+    <mergeCell ref="R39:W39"/>
     <mergeCell ref="R20:W20"/>
     <mergeCell ref="R19:W19"/>
     <mergeCell ref="B2:H2"/>
@@ -16283,11 +16283,6 @@
     <mergeCell ref="B12:H12"/>
     <mergeCell ref="J19:P19"/>
     <mergeCell ref="J20:P20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="J29:P29"/>
-    <mergeCell ref="R29:W29"/>
-    <mergeCell ref="J38:P38"/>
-    <mergeCell ref="R39:W39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18695,11 +18690,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="J29:P29"/>
-    <mergeCell ref="R29:W29"/>
-    <mergeCell ref="J38:P38"/>
-    <mergeCell ref="R39:W39"/>
     <mergeCell ref="J20:P20"/>
     <mergeCell ref="R20:W20"/>
     <mergeCell ref="B2:H2"/>
@@ -18707,6 +18697,11 @@
     <mergeCell ref="B12:H12"/>
     <mergeCell ref="J19:P19"/>
     <mergeCell ref="R19:W19"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="J29:P29"/>
+    <mergeCell ref="R29:W29"/>
+    <mergeCell ref="J38:P38"/>
+    <mergeCell ref="R39:W39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21293,15 +21288,15 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">H3*I3</f>
-        <v>9750000</v>
+        <v>8450000</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">I3-B3</f>
-        <v>5250000</v>
+        <v>4550000</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">B3-C3</f>
-        <v>4500000</v>
+        <v>3900000</v>
       </c>
       <c r="E3" s="5">
         <f t="shared" ref="E3:E8" ca="1" si="0">D3/B3</f>
@@ -21309,14 +21304,14 @@
       </c>
       <c r="F3" s="5">
         <f ca="1">B3/B8</f>
-        <v>0.24235645041014167</v>
+        <v>0.17304935490477166</v>
       </c>
       <c r="H3">
         <v>0.65</v>
       </c>
       <c r="I3" s="6">
         <f ca="1">RANDBETWEEN(10,15)*1000000</f>
-        <v>15000000</v>
+        <v>13000000</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -21325,15 +21320,15 @@
       </c>
       <c r="B4" s="2">
         <f t="shared" ref="B4:B7" ca="1" si="1">H4*I4</f>
-        <v>14880000</v>
+        <v>19680000</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:C7" ca="1" si="2">I4-B4</f>
-        <v>16120000</v>
+        <v>21320000</v>
       </c>
       <c r="D4" s="2">
         <f ca="1">B4-C4</f>
-        <v>-1240000</v>
+        <v>-1640000</v>
       </c>
       <c r="E4" s="5">
         <f t="shared" ca="1" si="0"/>
@@ -21341,14 +21336,14 @@
       </c>
       <c r="F4" s="5">
         <f ca="1">B4/B8</f>
-        <v>0.36987322893363161</v>
+        <v>0.40303092361253329</v>
       </c>
       <c r="H4">
         <v>0.48</v>
       </c>
       <c r="I4" s="6">
         <f ca="1">RANDBETWEEN(30,45)*1000000</f>
-        <v>31000000</v>
+        <v>41000000</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -21357,15 +21352,15 @@
       </c>
       <c r="B5" s="2">
         <f ca="1">H5*I5</f>
-        <v>2400000</v>
+        <v>4200000</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1600000</v>
+        <v>2800000</v>
       </c>
       <c r="D5" s="2">
         <f ca="1">B5-C5</f>
-        <v>800000</v>
+        <v>1400000</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" ca="1" si="0"/>
@@ -21373,14 +21368,14 @@
       </c>
       <c r="F5" s="5">
         <f ca="1">B5/B8</f>
-        <v>5.9656972408650262E-2</v>
+        <v>8.6012697112430883E-2</v>
       </c>
       <c r="H5">
         <v>0.6</v>
       </c>
       <c r="I5" s="6">
         <f ca="1">RANDBETWEEN(4,8)*1000000</f>
-        <v>4000000</v>
+        <v>7000000</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -21389,30 +21384,30 @@
       </c>
       <c r="B6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>11000000</v>
+        <v>13200000.000000002</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>9000000</v>
+        <v>10799999.999999998</v>
       </c>
       <c r="D6" s="2">
         <f ca="1">B6-C6</f>
-        <v>2000000</v>
+        <v>2400000.0000000037</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18181818181818182</v>
+        <v>0.18181818181818207</v>
       </c>
       <c r="F6" s="5">
         <f ca="1">B6/B8</f>
-        <v>0.27342779020631369</v>
+        <v>0.27032561949621137</v>
       </c>
       <c r="H6">
         <v>0.55000000000000004</v>
       </c>
       <c r="I6" s="6">
         <f ca="1">RANDBETWEEN(15,25)*1000000</f>
-        <v>20000000</v>
+        <v>24000000</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -21421,30 +21416,30 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>2200000</v>
+        <v>3300000.0000000005</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="2"/>
-        <v>1800000</v>
+        <v>2699999.9999999995</v>
       </c>
       <c r="D7" s="2">
         <f ca="1">B7-C7</f>
-        <v>400000</v>
+        <v>600000.00000000093</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18181818181818182</v>
+        <v>0.18181818181818207</v>
       </c>
       <c r="F7" s="5">
         <f ca="1">B7/B8</f>
-        <v>5.4685558041262738E-2</v>
+        <v>6.7581404874052842E-2</v>
       </c>
       <c r="H7">
         <v>0.55000000000000004</v>
       </c>
       <c r="I7" s="6">
         <f ca="1">RANDBETWEEN(3,6)*1000000</f>
-        <v>4000000</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -21453,19 +21448,19 @@
       </c>
       <c r="B8" s="3">
         <f ca="1">SUM(B3:B7)</f>
-        <v>40230000</v>
+        <v>48830000</v>
       </c>
       <c r="C8" s="3">
         <f ca="1">SUM(C3:C7)</f>
-        <v>33770000</v>
+        <v>42170000</v>
       </c>
       <c r="D8" s="3">
         <f ca="1">SUM(D3:D7)</f>
-        <v>6460000</v>
+        <v>6660000.0000000047</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16057668406661696</v>
+        <v>0.13639156256399765</v>
       </c>
       <c r="F8" s="5">
         <f ca="1">B8/B8</f>
@@ -21498,15 +21493,15 @@
       </c>
       <c r="B11" s="2">
         <f ca="1">H11*I11</f>
-        <v>8680000</v>
+        <v>7440000</v>
       </c>
       <c r="C11" s="2">
         <f ca="1">I11-B11</f>
-        <v>5320000</v>
+        <v>4560000</v>
       </c>
       <c r="D11" s="2">
         <f ca="1">B11-C11</f>
-        <v>3360000</v>
+        <v>2880000</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" ref="E11:E16" ca="1" si="3">D11/B11</f>
@@ -21514,14 +21509,14 @@
       </c>
       <c r="F11" s="5">
         <f ca="1">B11/B16</f>
-        <v>0.22307890002570033</v>
+        <v>0.17777777777777778</v>
       </c>
       <c r="H11">
         <v>0.62</v>
       </c>
       <c r="I11" s="6">
         <f ca="1">RANDBETWEEN(10,15)*1000000</f>
-        <v>14000000</v>
+        <v>12000000</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -21530,15 +21525,15 @@
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12:B15" ca="1" si="4">H12*I12</f>
-        <v>16660000</v>
+        <v>19110000</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" ref="C12:C15" ca="1" si="5">I12-B12</f>
-        <v>17340000</v>
+        <v>19890000</v>
       </c>
       <c r="D12" s="2">
         <f ca="1">B12-C12</f>
-        <v>-680000</v>
+        <v>-780000</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" ca="1" si="3"/>
@@ -21546,14 +21541,14 @@
       </c>
       <c r="F12" s="5">
         <f ca="1">B12/B16</f>
-        <v>0.42816756617836033</v>
+        <v>0.45663082437275987</v>
       </c>
       <c r="H12">
         <v>0.49</v>
       </c>
       <c r="I12" s="6">
         <f ca="1">RANDBETWEEN(30,45)*1000000</f>
-        <v>34000000</v>
+        <v>39000000</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -21562,15 +21557,15 @@
       </c>
       <c r="B13" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>2320000</v>
+        <v>4640000</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>1680000</v>
+        <v>3360000</v>
       </c>
       <c r="D13" s="2">
         <f ca="1">B13-C13</f>
-        <v>640000</v>
+        <v>1280000</v>
       </c>
       <c r="E13" s="5">
         <f t="shared" ca="1" si="3"/>
@@ -21578,14 +21573,14 @@
       </c>
       <c r="F13" s="5">
         <f ca="1">B13/B16</f>
-        <v>5.962477512207659E-2</v>
+        <v>0.11087216248506571</v>
       </c>
       <c r="H13">
         <v>0.57999999999999996</v>
       </c>
       <c r="I13" s="6">
         <f ca="1">RANDBETWEEN(4,8)*1000000</f>
-        <v>4000000</v>
+        <v>8000000</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -21594,15 +21589,15 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>7950000</v>
+        <v>9010000</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>7050000</v>
+        <v>7990000</v>
       </c>
       <c r="D14" s="2">
         <f ca="1">B14-C14</f>
-        <v>900000</v>
+        <v>1020000</v>
       </c>
       <c r="E14" s="5">
         <f t="shared" ca="1" si="3"/>
@@ -21610,14 +21605,14 @@
       </c>
       <c r="F14" s="5">
         <f ca="1">B14/B16</f>
-        <v>0.20431765612952968</v>
+        <v>0.21529271206690562</v>
       </c>
       <c r="H14">
         <v>0.53</v>
       </c>
       <c r="I14" s="6">
         <f ca="1">RANDBETWEEN(15,25)*1000000</f>
-        <v>15000000</v>
+        <v>17000000</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -21626,15 +21621,15 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>3300000.0000000005</v>
+        <v>1650000.0000000002</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>2699999.9999999995</v>
+        <v>1349999.9999999998</v>
       </c>
       <c r="D15" s="2">
         <f ca="1">B15-C15</f>
-        <v>600000.00000000093</v>
+        <v>300000.00000000047</v>
       </c>
       <c r="E15" s="5">
         <f t="shared" ca="1" si="3"/>
@@ -21642,14 +21637,14 @@
       </c>
       <c r="F15" s="5">
         <f ca="1">B15/B16</f>
-        <v>8.4811102544333092E-2</v>
+        <v>3.9426523297491044E-2</v>
       </c>
       <c r="H15">
         <v>0.55000000000000004</v>
       </c>
       <c r="I15" s="6">
         <f ca="1">RANDBETWEEN(3,6)*1000000</f>
-        <v>6000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -21658,19 +21653,19 @@
       </c>
       <c r="B16" s="3">
         <f ca="1">SUM(B11:B15)</f>
-        <v>38910000</v>
+        <v>41850000</v>
       </c>
       <c r="C16" s="3">
         <f ca="1">SUM(C11:C15)</f>
-        <v>34090000</v>
+        <v>37150000</v>
       </c>
       <c r="D16" s="3">
         <f ca="1">SUM(D11:D15)</f>
-        <v>4820000.0000000009</v>
+        <v>4700000</v>
       </c>
       <c r="E16" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>0.123875610382935</v>
+        <v>0.11230585424133811</v>
       </c>
       <c r="F16" s="5">
         <f ca="1">B16/B16</f>
@@ -21731,15 +21726,15 @@
       </c>
       <c r="B19" s="2">
         <f ca="1">B11-B3</f>
-        <v>-1070000</v>
+        <v>-1010000</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" ref="C19:C23" ca="1" si="6">C11-C3</f>
-        <v>70000</v>
+        <v>10000</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" ref="D19" ca="1" si="7">D11-D3</f>
-        <v>-1140000</v>
+        <v>-1020000</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" ref="E19:F19" ca="1" si="8">E11-E3</f>
@@ -21747,23 +21742,23 @@
       </c>
       <c r="F19" s="5">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.9277550384441344E-2</v>
+        <v>4.7284228730061217E-3</v>
       </c>
       <c r="H19" s="2">
         <f ca="1">F3*$B$8*E19</f>
-        <v>-725806.45161290362</v>
+        <v>-629032.25806451647</v>
       </c>
       <c r="I19" s="4">
         <f ca="1">$B$8*E11*F19</f>
-        <v>-300207.42656751297</v>
+        <v>89376.34408602152</v>
       </c>
       <c r="J19" s="4">
         <f ca="1">E11*F11*$B$24</f>
-        <v>-113986.12181958361</v>
+        <v>-480344.08602150553</v>
       </c>
       <c r="K19" s="3">
         <f ca="1">SUM(H19:J19)</f>
-        <v>-1140000.0000000002</v>
+        <v>-1020000.0000000005</v>
       </c>
       <c r="L19" s="3">
         <f ca="1">K19-D19</f>
@@ -21780,15 +21775,15 @@
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" ca="1" si="9">B12-B4</f>
-        <v>1780000</v>
+        <v>-570000</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>1220000</v>
+        <v>-1430000</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" ref="D20" ca="1" si="10">D12-D4</f>
-        <v>560000</v>
+        <v>860000</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" ref="E20:F20" ca="1" si="11">E12-E4</f>
@@ -21796,23 +21791,23 @@
       </c>
       <c r="F20" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>5.8294337244728711E-2</v>
+        <v>5.3599900760226582E-2</v>
       </c>
       <c r="H20" s="2">
         <f ca="1">F4*$B$8*E20</f>
-        <v>632653.06122448982</v>
+        <v>836734.69387755101</v>
       </c>
       <c r="I20" s="4">
         <f t="shared" ref="I20:I23" ca="1" si="12">$B$8*E12*F20</f>
-        <v>-95721.681116548396</v>
+        <v>-106827.88384170872</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" ref="J20:J23" ca="1" si="13">E12*F12*$B$24</f>
-        <v>23068.619892058588</v>
+        <v>130093.18996415773</v>
       </c>
       <c r="K20" s="3">
         <f t="shared" ref="K20:K24" ca="1" si="14">SUM(H20:J20)</f>
-        <v>560000</v>
+        <v>860000</v>
       </c>
       <c r="L20" s="3">
         <f t="shared" ref="L20:L24" ca="1" si="15">K20-D20</f>
@@ -21829,15 +21824,15 @@
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" ca="1" si="17">B13-B5</f>
-        <v>-80000</v>
+        <v>440000</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>80000</v>
+        <v>560000</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" ref="D21" ca="1" si="18">D13-D5</f>
-        <v>-160000</v>
+        <v>-120000</v>
       </c>
       <c r="E21" s="5">
         <f t="shared" ref="E21:F21" ca="1" si="19">E13-E5</f>
@@ -21845,23 +21840,23 @@
       </c>
       <c r="F21" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-3.2197286573672212E-5</v>
+        <v>2.4859465372634823E-2</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" ref="H21:H23" ca="1" si="20">F5*$B$8*E21</f>
-        <v>-137931.03448275858</v>
+        <v>-241379.31034482754</v>
       </c>
       <c r="I21" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>-357.32326589209191</v>
+        <v>334865.5707988299</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-21711.642251349262</v>
+        <v>-213486.26045400245</v>
       </c>
       <c r="K21" s="3">
         <f t="shared" ca="1" si="14"/>
-        <v>-159999.99999999994</v>
+        <v>-120000.00000000009</v>
       </c>
       <c r="L21" s="3">
         <f t="shared" ca="1" si="15"/>
@@ -21878,39 +21873,39 @@
       </c>
       <c r="B22" s="2">
         <f t="shared" ref="B22" ca="1" si="21">B14-B6</f>
-        <v>-3050000</v>
+        <v>-4190000.0000000019</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>-1950000</v>
+        <v>-2809999.9999999981</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" ref="D22" ca="1" si="22">D14-D6</f>
-        <v>-1100000</v>
+        <v>-1380000.0000000037</v>
       </c>
       <c r="E22" s="5">
         <f t="shared" ref="E22:F22" ca="1" si="23">E14-E6</f>
-        <v>-6.86106346483705E-2</v>
+        <v>-6.861063464837075E-2</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" ca="1" si="23"/>
-        <v>-6.9110134076784013E-2</v>
+        <v>-5.503290742930575E-2</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" ca="1" si="20"/>
-        <v>-754716.98113207554</v>
+        <v>-905660.37735849398</v>
       </c>
       <c r="I22" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>-314751.02195196465</v>
+        <v>-304217.75884222641</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-30531.996915959895</v>
+        <v>-170121.86379928322</v>
       </c>
       <c r="K22" s="3">
         <f t="shared" ca="1" si="14"/>
-        <v>-1100000.0000000002</v>
+        <v>-1380000.0000000037</v>
       </c>
       <c r="L22" s="3">
         <f t="shared" ca="1" si="15"/>
@@ -21927,39 +21922,39 @@
       </c>
       <c r="B23" s="2">
         <f t="shared" ref="B23" ca="1" si="24">B15-B7</f>
-        <v>1100000.0000000005</v>
+        <v>-1650000.0000000002</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>899999.99999999953</v>
+        <v>-1349999.9999999998</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" ref="D23" ca="1" si="25">D15-D7</f>
-        <v>200000.00000000093</v>
+        <v>-300000.00000000047</v>
       </c>
       <c r="E23" s="5">
         <f t="shared" ref="E23:F23" ca="1" si="26">E15-E7</f>
-        <v>2.4980018054066022E-16</v>
+        <v>0</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" ca="1" si="26"/>
-        <v>3.0125544503070353E-2</v>
+        <v>-2.8154881576561798E-2</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" ca="1" si="20"/>
-        <v>5.4956039718945249E-10</v>
+        <v>0</v>
       </c>
       <c r="I23" s="4">
         <f t="shared" ca="1" si="12"/>
-        <v>220354.66461064035</v>
+        <v>-249964.15770609357</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" ca="1" si="13"/>
-        <v>-20354.664610639964</v>
+        <v>-50035.842293906899</v>
       </c>
       <c r="K23" s="3">
         <f t="shared" ca="1" si="14"/>
-        <v>200000.00000000093</v>
+        <v>-300000.00000000047</v>
       </c>
       <c r="L23" s="3">
         <f t="shared" ca="1" si="15"/>
@@ -21976,19 +21971,19 @@
       </c>
       <c r="B24" s="3">
         <f ca="1">SUM(B19:B23)</f>
-        <v>-1319999.9999999995</v>
+        <v>-6980000.0000000019</v>
       </c>
       <c r="C24" s="3">
         <f ca="1">SUM(C19:C23)</f>
-        <v>319999.99999999953</v>
+        <v>-5019999.9999999981</v>
       </c>
       <c r="D24" s="3">
         <f ca="1">SUM(D19:D23)</f>
-        <v>-1639999.9999999991</v>
+        <v>-1960000.0000000042</v>
       </c>
       <c r="E24" s="5">
         <f t="shared" ref="E24:F24" ca="1" si="27">E16-E8</f>
-        <v>-3.6701073683681959E-2</v>
+        <v>-2.4085708322659535E-2</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" ca="1" si="27"/>
@@ -21996,19 +21991,19 @@
       </c>
       <c r="H24" s="4">
         <f ca="1">SUM(H19:H23)</f>
-        <v>-985801.40600324736</v>
+        <v>-939337.25189028704</v>
       </c>
       <c r="I24" s="4">
         <f ca="1">SUM(I19:I23)</f>
-        <v>-490682.78829127783</v>
+        <v>-236767.88550517731</v>
       </c>
       <c r="J24" s="4">
         <f ca="1">SUM(J19:J23)</f>
-        <v>-163515.80570547414</v>
+        <v>-783894.86260454031</v>
       </c>
       <c r="K24" s="3">
         <f t="shared" ca="1" si="14"/>
-        <v>-1639999.9999999995</v>
+        <v>-1960000.0000000047</v>
       </c>
       <c r="L24" s="3">
         <f t="shared" ca="1" si="15"/>
@@ -22026,37 +22021,37 @@
       </c>
       <c r="D26" s="10">
         <f t="shared" ref="D26:D31" ca="1" si="28">E3*F3</f>
-        <v>0.11185682326621924</v>
+        <v>7.9868933032971545E-2</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D27" s="10">
         <f t="shared" ca="1" si="28"/>
-        <v>-3.0822769077802632E-2</v>
+        <v>-3.3585910301044436E-2</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D28" s="10">
         <f t="shared" ca="1" si="28"/>
-        <v>1.9885657469550087E-2</v>
+        <v>2.8670899037476959E-2</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D29" s="10">
         <f t="shared" ca="1" si="28"/>
-        <v>4.9714143673875215E-2</v>
+        <v>4.9150112635674863E-2</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D30" s="10">
         <f t="shared" ca="1" si="28"/>
-        <v>9.9428287347750437E-3</v>
+        <v>1.2287528158918716E-2</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D31" s="10">
         <f t="shared" ca="1" si="28"/>
-        <v>0.16057668406661696</v>
+        <v>0.13639156256399765</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.25">
@@ -22065,37 +22060,37 @@
       </c>
       <c r="D34" s="10">
         <f t="shared" ref="D34:D39" ca="1" si="29">E11*F11</f>
-        <v>8.6353122590593676E-2</v>
+        <v>6.8817204301075269E-2</v>
       </c>
     </row>
     <row r="35" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D35" s="10">
         <f t="shared" ca="1" si="29"/>
-        <v>-1.7476227190953483E-2</v>
+        <v>-1.8637992831541217E-2</v>
       </c>
     </row>
     <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D36" s="10">
         <f t="shared" ca="1" si="29"/>
-        <v>1.6448213826779749E-2</v>
+        <v>3.0585424133811229E-2</v>
       </c>
     </row>
     <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D37" s="10">
         <f t="shared" ca="1" si="29"/>
-        <v>2.313030069390902E-2</v>
+        <v>2.4372759856630826E-2</v>
       </c>
     </row>
     <row r="38" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D38" s="10">
         <f t="shared" ca="1" si="29"/>
-        <v>1.5420200462606039E-2</v>
+        <v>7.1684587813620176E-3</v>
       </c>
     </row>
     <row r="39" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D39" s="10">
         <f t="shared" ca="1" si="29"/>
-        <v>0.123875610382935</v>
+        <v>0.11230585424133811</v>
       </c>
     </row>
     <row r="41" spans="3:8" x14ac:dyDescent="0.25">
@@ -22118,19 +22113,19 @@
       </c>
       <c r="D42" s="10">
         <f ca="1">D34-D26</f>
-        <v>-2.550370067562556E-2</v>
+        <v>-1.1051728731896276E-2</v>
       </c>
       <c r="E42" s="10">
         <f ca="1">E19*F3</f>
-        <v>-1.8041423107454723E-2</v>
+        <v>-1.2882085973059931E-2</v>
       </c>
       <c r="F42" s="10">
         <f ca="1">F19*E3</f>
-        <v>-8.897330946665236E-3</v>
+        <v>2.1823490183105177E-3</v>
       </c>
       <c r="G42" s="10">
         <f ca="1">E19*F19</f>
-        <v>1.4350533784943935E-3</v>
+        <v>-3.5199177714685789E-4</v>
       </c>
       <c r="H42" s="1">
         <f ca="1">SUM(E42:G42)-D42</f>
@@ -22140,19 +22135,19 @@
     <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D43" s="10">
         <f t="shared" ref="D43:D47" ca="1" si="30">D35-D27</f>
-        <v>1.334654188684915E-2</v>
+        <v>1.4947917469503219E-2</v>
       </c>
       <c r="E43" s="10">
         <f t="shared" ref="E43:E47" ca="1" si="31">E20*F4</f>
-        <v>1.5725902590715629E-2</v>
+        <v>1.713566852094104E-2</v>
       </c>
       <c r="F43" s="10">
         <f t="shared" ref="F43:F47" ca="1" si="32">F20*E4</f>
-        <v>-4.8578614370607259E-3</v>
+        <v>-4.4666583966855482E-3</v>
       </c>
       <c r="G43" s="10">
         <f t="shared" ref="G43:G47" ca="1" si="33">E20*F20</f>
-        <v>2.4785007331942477E-3</v>
+        <v>2.2789073452477286E-3</v>
       </c>
       <c r="H43" s="1">
         <f t="shared" ref="H43:H47" ca="1" si="34">SUM(E43:G43)-D43</f>
@@ -22162,19 +22157,19 @@
     <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D44" s="10">
         <f t="shared" ca="1" si="30"/>
-        <v>-3.4374436427703388E-3</v>
+        <v>1.9145250963342707E-3</v>
       </c>
       <c r="E44" s="10">
         <f t="shared" ca="1" si="31"/>
-        <v>-3.4285616326810487E-3</v>
+        <v>-4.9432584547374056E-3</v>
       </c>
       <c r="F44" s="10">
         <f t="shared" ca="1" si="32"/>
-        <v>-1.0732428857890736E-5</v>
+        <v>8.286488457544941E-3</v>
       </c>
       <c r="G44" s="10">
         <f t="shared" ca="1" si="33"/>
-        <v>1.8504187686018508E-6</v>
+        <v>-1.4287049064732654E-3</v>
       </c>
       <c r="H44" s="1">
         <f t="shared" ca="1" si="34"/>
@@ -22184,19 +22179,19 @@
     <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D45" s="10">
         <f t="shared" ca="1" si="30"/>
-        <v>-2.6583842979966195E-2</v>
+        <v>-2.4777352779044037E-2</v>
       </c>
       <c r="E45" s="10">
         <f t="shared" ca="1" si="31"/>
-        <v>-1.8760054216556687E-2</v>
+        <v>-1.8547212315349046E-2</v>
       </c>
       <c r="F45" s="10">
         <f t="shared" ca="1" si="32"/>
-        <v>-1.2565478923051638E-2</v>
+        <v>-1.0005983168964696E-2</v>
       </c>
       <c r="G45" s="10">
         <f ca="1">E22*F22</f>
-        <v>4.7416901596421283E-3</v>
+        <v>3.7758427052697052E-3</v>
       </c>
       <c r="H45" s="1">
         <f t="shared" ca="1" si="34"/>
@@ -22206,19 +22201,19 @@
     <row r="46" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D46" s="10">
         <f t="shared" ca="1" si="30"/>
-        <v>5.4773717278309951E-3</v>
+        <v>-5.1190693775566981E-3</v>
       </c>
       <c r="E46" s="10">
         <f t="shared" ca="1" si="31"/>
-        <v>1.3660462271674185E-17</v>
+        <v>0</v>
       </c>
       <c r="F46" s="10">
         <f t="shared" ca="1" si="32"/>
-        <v>5.4773717278309734E-3</v>
+        <v>-5.1190693775566981E-3</v>
       </c>
       <c r="G46" s="10">
         <f t="shared" ca="1" si="33"/>
-        <v>7.5253664557526688E-18</v>
+        <v>0</v>
       </c>
       <c r="H46" s="1">
         <f t="shared" ca="1" si="34"/>
@@ -22228,11 +22223,11 @@
     <row r="47" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D47" s="10">
         <f t="shared" ca="1" si="30"/>
-        <v>-3.6701073683681959E-2</v>
+        <v>-2.4085708322659535E-2</v>
       </c>
       <c r="E47" s="10">
         <f t="shared" ca="1" si="31"/>
-        <v>-3.6701073683681959E-2</v>
+        <v>-2.4085708322659535E-2</v>
       </c>
       <c r="F47" s="10">
         <f t="shared" ca="1" si="32"/>
@@ -22343,19 +22338,19 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">K3*L3</f>
-        <v>11940000</v>
+        <v>9950000</v>
       </c>
       <c r="C3" s="2">
         <f ca="1">L3-B3</f>
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">SUM(B3:C3)</f>
-        <v>12000000</v>
+        <v>10000000</v>
       </c>
       <c r="E3" s="2">
         <f ca="1">B3-C3</f>
-        <v>11880000</v>
+        <v>9900000</v>
       </c>
       <c r="F3" s="5">
         <f ca="1">E3/D3</f>
@@ -22367,18 +22362,18 @@
       </c>
       <c r="H3" s="5">
         <f ca="1">D3/D8</f>
-        <v>0.13953488372093023</v>
+        <v>0.13157894736842105</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">B3/B8</f>
-        <v>0.2369047619047619</v>
+        <v>0.22644515248065544</v>
       </c>
       <c r="K3" s="7">
         <v>0.995</v>
       </c>
       <c r="L3" s="6">
         <f ca="1">RANDBETWEEN(10,15)*1000000</f>
-        <v>12000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -22387,19 +22382,19 @@
       </c>
       <c r="B4" s="2">
         <f t="shared" ref="B4:B7" ca="1" si="0">K4*L4</f>
-        <v>17760000</v>
+        <v>18240000</v>
       </c>
       <c r="C4" s="2">
         <f ca="1">L4-B4</f>
-        <v>19240000</v>
+        <v>19760000</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" ref="D4:D8" ca="1" si="1">SUM(B4:C4)</f>
-        <v>37000000</v>
+        <v>38000000</v>
       </c>
       <c r="E4" s="2">
         <f ca="1">B4-C4</f>
-        <v>-1480000</v>
+        <v>-1520000</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" ref="F4:F8" ca="1" si="2">E4/D4</f>
@@ -22411,18 +22406,18 @@
       </c>
       <c r="H4" s="5">
         <f ca="1">D4/D8</f>
-        <v>0.43023255813953487</v>
+        <v>0.5</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">B4/B8</f>
-        <v>0.35238095238095241</v>
+        <v>0.41511151570323168</v>
       </c>
       <c r="K4" s="7">
         <v>0.48</v>
       </c>
       <c r="L4" s="6">
         <f ca="1">RANDBETWEEN(30,45)*1000000</f>
-        <v>37000000</v>
+        <v>38000000</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -22455,11 +22450,11 @@
       </c>
       <c r="H5" s="5">
         <f ca="1">D5/D8</f>
-        <v>8.1395348837209308E-2</v>
+        <v>9.2105263157894732E-2</v>
       </c>
       <c r="I5" s="5">
         <f ca="1">B5/B8</f>
-        <v>8.3333333333333329E-2</v>
+        <v>9.5584888484296762E-2</v>
       </c>
       <c r="K5" s="7">
         <v>0.6</v>
@@ -22475,42 +22470,42 @@
       </c>
       <c r="B6" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>13750000.000000002</v>
+        <v>9900000</v>
       </c>
       <c r="C6" s="2">
         <f ca="1">L6-B6</f>
-        <v>11249999.999999998</v>
+        <v>8100000</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>25000000</v>
+        <v>18000000</v>
       </c>
       <c r="E6" s="2">
         <f ca="1">B6-C6</f>
-        <v>2500000.0000000037</v>
+        <v>1800000</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.10000000000000014</v>
+        <v>0.1</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>0.18181818181818207</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="H6" s="5">
         <f ca="1">D6/D8</f>
-        <v>0.29069767441860467</v>
+        <v>0.23684210526315788</v>
       </c>
       <c r="I6" s="5">
         <f ca="1">B6/B8</f>
-        <v>0.27281746031746035</v>
+        <v>0.22530723714155668</v>
       </c>
       <c r="K6" s="7">
         <v>0.55000000000000004</v>
       </c>
       <c r="L6" s="6">
         <f ca="1">RANDBETWEEN(15,25)*1000000</f>
-        <v>25000000</v>
+        <v>18000000</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -22519,42 +22514,42 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>2750000</v>
+        <v>1650000.0000000002</v>
       </c>
       <c r="C7" s="2">
         <f ca="1">L7-B7</f>
-        <v>2250000</v>
+        <v>1349999.9999999998</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
       <c r="E7" s="2">
         <f ca="1">B7-C7</f>
-        <v>500000</v>
+        <v>300000.00000000047</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.1</v>
+        <v>0.10000000000000016</v>
       </c>
       <c r="G7" s="5">
         <f ca="1">E7/B7</f>
-        <v>0.18181818181818182</v>
+        <v>0.18181818181818207</v>
       </c>
       <c r="H7" s="5">
         <f ca="1">D7/D8</f>
-        <v>5.8139534883720929E-2</v>
+        <v>3.9473684210526314E-2</v>
       </c>
       <c r="I7" s="5">
         <f ca="1">B7/B8</f>
-        <v>5.4563492063492064E-2</v>
+        <v>3.7551206190259451E-2</v>
       </c>
       <c r="K7" s="7">
         <v>0.55000000000000004</v>
       </c>
       <c r="L7" s="6">
         <f ca="1">RANDBETWEEN(3,6)*1000000</f>
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -22563,27 +22558,27 @@
       </c>
       <c r="B8" s="3">
         <f ca="1">SUM(B3:B7)</f>
-        <v>50400000</v>
+        <v>43940000</v>
       </c>
       <c r="C8" s="3">
         <f ca="1">SUM(C3:C7)</f>
-        <v>35600000</v>
+        <v>32060000</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" ca="1" si="1"/>
-        <v>86000000</v>
+        <v>76000000</v>
       </c>
       <c r="E8" s="3">
         <f ca="1">SUM(E3:E7)</f>
-        <v>14800000.000000004</v>
+        <v>11880000</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>0.17209302325581399</v>
+        <v>0.15631578947368421</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>0.29365079365079372</v>
+        <v>0.27036868456986801</v>
       </c>
       <c r="H8" s="5">
         <f ca="1">D8/D8</f>
@@ -22635,19 +22630,19 @@
       </c>
       <c r="B11" s="2">
         <f ca="1">K11*L11</f>
-        <v>9100000</v>
+        <v>10920000</v>
       </c>
       <c r="C11" s="2">
         <f ca="1">L11-B11</f>
-        <v>900000</v>
+        <v>1080000</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" ref="D11:D16" ca="1" si="4">SUM(B11:C11)</f>
-        <v>10000000</v>
+        <v>12000000</v>
       </c>
       <c r="E11" s="2">
         <f ca="1">B11-C11</f>
-        <v>8200000</v>
+        <v>9840000</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" ref="F11:F16" ca="1" si="5">E11/D11</f>
@@ -22659,18 +22654,18 @@
       </c>
       <c r="H11" s="5">
         <f ca="1">D11/D16</f>
-        <v>0.13333333333333333</v>
+        <v>0.14457831325301204</v>
       </c>
       <c r="I11" s="5">
         <f ca="1">B11/B16</f>
-        <v>0.21431935939707961</v>
+        <v>0.22999157540016849</v>
       </c>
       <c r="K11" s="7">
         <v>0.91</v>
       </c>
       <c r="L11" s="6">
         <f ca="1">RANDBETWEEN(10,15)*1000000</f>
-        <v>10000000</v>
+        <v>12000000</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -22679,19 +22674,19 @@
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12:B15" ca="1" si="6">K12*L12</f>
-        <v>18130000</v>
+        <v>19110000</v>
       </c>
       <c r="C12" s="2">
         <f ca="1">L12-B12</f>
-        <v>18870000</v>
+        <v>19890000</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>37000000</v>
+        <v>39000000</v>
       </c>
       <c r="E12" s="2">
         <f ca="1">B12-C12</f>
-        <v>-740000</v>
+        <v>-780000</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ca="1" si="5"/>
@@ -22703,18 +22698,18 @@
       </c>
       <c r="H12" s="5">
         <f ca="1">D12/D16</f>
-        <v>0.49333333333333335</v>
+        <v>0.46987951807228917</v>
       </c>
       <c r="I12" s="5">
         <f ca="1">B12/B16</f>
-        <v>0.42699010833725859</v>
+        <v>0.40248525695029486</v>
       </c>
       <c r="K12" s="7">
         <v>0.49</v>
       </c>
       <c r="L12" s="6">
         <f ca="1">RANDBETWEEN(30,45)*1000000</f>
-        <v>37000000</v>
+        <v>39000000</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -22723,42 +22718,42 @@
       </c>
       <c r="B13" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>3479999.9999999995</v>
+        <v>4640000</v>
       </c>
       <c r="C13" s="2">
         <f ca="1">L13-B13</f>
-        <v>2520000.0000000005</v>
+        <v>3360000</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>6000000</v>
+        <v>8000000</v>
       </c>
       <c r="E13" s="2">
         <f ca="1">B13-C13</f>
-        <v>959999.99999999907</v>
+        <v>1280000</v>
       </c>
       <c r="F13" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>0.15999999999999984</v>
+        <v>0.16</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>0.27586206896551702</v>
+        <v>0.27586206896551724</v>
       </c>
       <c r="H13" s="5">
         <f ca="1">D13/D16</f>
-        <v>0.08</v>
+        <v>9.6385542168674704E-2</v>
       </c>
       <c r="I13" s="5">
         <f ca="1">B13/B16</f>
-        <v>8.1959491285916147E-2</v>
+        <v>9.7725358045492844E-2</v>
       </c>
       <c r="K13" s="7">
         <v>0.57999999999999996</v>
       </c>
       <c r="L13" s="6">
         <f ca="1">RANDBETWEEN(4,8)*1000000</f>
-        <v>6000000</v>
+        <v>8000000</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -22767,19 +22762,19 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>10070000</v>
+        <v>11130000</v>
       </c>
       <c r="C14" s="2">
         <f ca="1">L14-B14</f>
-        <v>8930000</v>
+        <v>9870000</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>19000000</v>
+        <v>21000000</v>
       </c>
       <c r="E14" s="2">
         <f ca="1">B14-C14</f>
-        <v>1140000</v>
+        <v>1260000</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" ca="1" si="5"/>
@@ -22791,18 +22786,18 @@
       </c>
       <c r="H14" s="5">
         <f ca="1">D14/D16</f>
-        <v>0.25333333333333335</v>
+        <v>0.25301204819277107</v>
       </c>
       <c r="I14" s="5">
         <f ca="1">B14/B16</f>
-        <v>0.23716439001413095</v>
+        <v>0.23441449031171019</v>
       </c>
       <c r="K14" s="7">
         <v>0.53</v>
       </c>
       <c r="L14" s="6">
         <f ca="1">RANDBETWEEN(15,25)*1000000</f>
-        <v>19000000</v>
+        <v>21000000</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -22835,11 +22830,11 @@
       </c>
       <c r="H15" s="5">
         <f ca="1">D15/D16</f>
-        <v>0.04</v>
+        <v>3.614457831325301E-2</v>
       </c>
       <c r="I15" s="5">
         <f ca="1">B15/B16</f>
-        <v>3.9566650965614701E-2</v>
+        <v>3.5383319292333619E-2</v>
       </c>
       <c r="K15" s="7">
         <v>0.56000000000000005</v>
@@ -22855,27 +22850,27 @@
       </c>
       <c r="B16" s="3">
         <f ca="1">SUM(B11:B15)</f>
-        <v>42460000</v>
+        <v>47480000</v>
       </c>
       <c r="C16" s="3">
         <f ca="1">SUM(C11:C15)</f>
-        <v>32540000</v>
+        <v>35520000</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" ca="1" si="4"/>
-        <v>75000000</v>
+        <v>83000000</v>
       </c>
       <c r="E16" s="3">
         <f ca="1">SUM(E11:E15)</f>
-        <v>9920000</v>
+        <v>11960000</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>0.13226666666666667</v>
+        <v>0.14409638554216866</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>0.23363165332077249</v>
+        <v>0.25189553496208927</v>
       </c>
       <c r="H16" s="5">
         <f ca="1">D16/D16</f>
@@ -22975,19 +22970,19 @@
       </c>
       <c r="B19" s="2">
         <f ca="1">B11-B3</f>
-        <v>-2840000</v>
+        <v>970000</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" ref="C19:F24" ca="1" si="8">C11-C3</f>
-        <v>840000</v>
+        <v>1030000</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" ref="D19" ca="1" si="9">D11-D3</f>
-        <v>-2000000</v>
+        <v>2000000</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>-3680000</v>
+        <v>-60000</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" ca="1" si="8"/>
@@ -22999,59 +22994,59 @@
       </c>
       <c r="H19" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>-6.2015503875968991E-3</v>
+        <v>1.2999365884590997E-2</v>
       </c>
       <c r="I19" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>-2.258540250768229E-2</v>
+        <v>3.5464229195130426E-3</v>
       </c>
       <c r="K19" s="2">
         <f ca="1">H3*$D$8*F19</f>
-        <v>-2040000.0000000005</v>
+        <v>-1700000.0000000005</v>
       </c>
       <c r="L19" s="3">
         <f ca="1">$D$8*F3*H19</f>
-        <v>-528000</v>
+        <v>978072.28915662656</v>
       </c>
       <c r="M19" s="3">
         <f ca="1">F3*H3*$D$24</f>
-        <v>-1519534.8837209304</v>
+        <v>911842.10526315786</v>
       </c>
       <c r="N19" s="3">
         <f ca="1">SUM(K19:M19)</f>
-        <v>-4087534.8837209307</v>
+        <v>189914.39441978396</v>
       </c>
       <c r="O19" s="3">
         <f t="shared" ref="O19:O24" ca="1" si="11">N19-E19</f>
-        <v>-407534.88372093067</v>
+        <v>249914.39441978396</v>
       </c>
       <c r="P19" s="5">
         <f t="shared" ref="P19:P24" ca="1" si="12">O19/E19</f>
-        <v>0.11074317492416594</v>
+        <v>-4.1652399069963995</v>
       </c>
       <c r="R19" s="2">
         <f ca="1">H27*$D$8*F43</f>
-        <v>2040000.0000000005</v>
+        <v>1700000.0000000005</v>
       </c>
       <c r="S19" s="3">
         <f ca="1">$C$8*F27*H43</f>
-        <v>218567.4418604651</v>
+        <v>-412592.07355738746</v>
       </c>
       <c r="T19" s="3">
         <f ca="1">F27*H27*$C$24</f>
-        <v>422706.97674418584</v>
+        <v>-450710.52631578944</v>
       </c>
       <c r="U19" s="3">
         <f ca="1">SUM(R19:T19)</f>
-        <v>2681274.418604651</v>
+        <v>836697.40012682346</v>
       </c>
       <c r="V19" s="3">
         <f ca="1">U19+E19</f>
-        <v>-998725.581395349</v>
+        <v>776697.40012682346</v>
       </c>
       <c r="W19" s="5">
         <f ca="1">V19/-E19</f>
-        <v>-0.27139282103134482</v>
+        <v>12.944956668780391</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
@@ -23060,15 +23055,15 @@
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20:B23" ca="1" si="13">B12-B4</f>
-        <v>370000</v>
+        <v>870000</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>-370000</v>
+        <v>130000</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" ref="D20" ca="1" si="14">D12-D4</f>
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" ca="1" si="8"/>
@@ -23084,59 +23079,59 @@
       </c>
       <c r="H20" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>6.3100775193798475E-2</v>
+        <v>-3.0120481927710829E-2</v>
       </c>
       <c r="I20" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>7.4609155956306183E-2</v>
+        <v>-1.2626258752936825E-2</v>
       </c>
       <c r="K20" s="2">
         <f ca="1">H4*$D$8*F20</f>
-        <v>740000</v>
+        <v>760000</v>
       </c>
       <c r="L20" s="3">
         <f t="shared" ref="L20:L23" ca="1" si="16">$D$8*F4*H20</f>
-        <v>-217066.66666666674</v>
+        <v>91566.265060240927</v>
       </c>
       <c r="M20" s="3">
         <f t="shared" ref="M20:M23" ca="1" si="17">F4*H4*$D$24</f>
-        <v>189302.32558139533</v>
+        <v>-140000</v>
       </c>
       <c r="N20" s="3">
         <f t="shared" ref="N20:N24" ca="1" si="18">SUM(K20:M20)</f>
-        <v>712235.65891472856</v>
+        <v>711566.26506024087</v>
       </c>
       <c r="O20" s="3">
         <f t="shared" ca="1" si="11"/>
-        <v>-27764.341085271444</v>
+        <v>-28433.734939759132</v>
       </c>
       <c r="P20" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>-3.7519379844961412E-2</v>
+        <v>-3.842396613480964E-2</v>
       </c>
       <c r="R20" s="2">
         <f t="shared" ref="R20:R23" ca="1" si="19">H28*$D$8*F44</f>
-        <v>-740000</v>
+        <v>-760000</v>
       </c>
       <c r="S20" s="3">
         <f t="shared" ref="S20:S23" ca="1" si="20">$C$8*F28*H44</f>
-        <v>89855.503875969021</v>
+        <v>-38626.506024096365</v>
       </c>
       <c r="T20" s="3">
         <f t="shared" ref="T20:T23" ca="1" si="21">F28*H28*$C$24</f>
-        <v>-52660.465116279032</v>
+        <v>69200</v>
       </c>
       <c r="U20" s="3">
         <f t="shared" ref="U20:U24" ca="1" si="22">SUM(R20:T20)</f>
-        <v>-702804.96124031011</v>
+        <v>-729426.50602409639</v>
       </c>
       <c r="V20" s="3">
         <f t="shared" ref="V20:V24" ca="1" si="23">U20+E20</f>
-        <v>37195.038759689895</v>
+        <v>10573.493975903606</v>
       </c>
       <c r="W20" s="5">
         <f t="shared" ref="W20:W24" ca="1" si="24">V20/-E20</f>
-        <v>-5.0263565891472829E-2</v>
+        <v>-1.4288505372842712E-2</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
@@ -23145,83 +23140,83 @@
       </c>
       <c r="B21" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>-720000.00000000047</v>
+        <v>440000</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>-279999.99999999953</v>
+        <v>560000</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" ref="D21" ca="1" si="25">D13-D5</f>
-        <v>-1000000</v>
+        <v>1000000</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>-440000.00000000093</v>
+        <v>-120000</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.0000000000000174E-2</v>
+        <v>-4.0000000000000008E-2</v>
       </c>
       <c r="G21" s="5">
         <f t="shared" ref="G21" ca="1" si="26">G13-G5</f>
-        <v>-5.7471264367816299E-2</v>
+        <v>-5.7471264367816077E-2</v>
       </c>
       <c r="H21" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>-1.3953488372093065E-3</v>
+        <v>4.2802790107799721E-3</v>
       </c>
       <c r="I21" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>-1.3738420474171814E-3</v>
+        <v>2.1404695611960817E-3</v>
       </c>
       <c r="K21" s="2">
         <f ca="1">H5*$D$8*F21</f>
-        <v>-280000.00000000128</v>
+        <v>-280000.00000000006</v>
       </c>
       <c r="L21" s="3">
         <f t="shared" ca="1" si="16"/>
-        <v>-24000.000000000073</v>
+        <v>65060.240963855576</v>
       </c>
       <c r="M21" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>-179069.76744186049</v>
+        <v>128947.36842105263</v>
       </c>
       <c r="N21" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>-483069.7674418618</v>
+        <v>-85992.390615091848</v>
       </c>
       <c r="O21" s="3">
         <f t="shared" ca="1" si="11"/>
-        <v>-43069.767441860866</v>
+        <v>34007.609384908152</v>
       </c>
       <c r="P21" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>9.7885835095138124E-2</v>
+        <v>-0.28339674487423461</v>
       </c>
       <c r="R21" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>280000.00000000128</v>
+        <v>280000.00000000006</v>
       </c>
       <c r="S21" s="3">
         <f t="shared" ca="1" si="20"/>
-        <v>9934.8837209302619</v>
+        <v>-27445.149017121181</v>
       </c>
       <c r="T21" s="3">
         <f t="shared" ca="1" si="21"/>
-        <v>49813.95348837207</v>
+        <v>-63736.842105263153</v>
       </c>
       <c r="U21" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>339748.83720930363</v>
+        <v>188818.00887761574</v>
       </c>
       <c r="V21" s="3">
         <f t="shared" ca="1" si="23"/>
-        <v>-100251.1627906973</v>
+        <v>68818.008877615735</v>
       </c>
       <c r="W21" s="5">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.22784355179703883</v>
+        <v>0.57348340731346448</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
@@ -23230,83 +23225,83 @@
       </c>
       <c r="B22" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>-3680000.0000000019</v>
+        <v>1230000</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>-2319999.9999999981</v>
+        <v>1770000</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" ref="D22" ca="1" si="27">D14-D6</f>
-        <v>-6000000</v>
+        <v>3000000</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>-1360000.0000000037</v>
+        <v>-540000</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" ca="1" si="8"/>
-        <v>-4.0000000000000147E-2</v>
+        <v>-4.0000000000000008E-2</v>
       </c>
       <c r="G22" s="5">
         <f t="shared" ref="G22" ca="1" si="28">G14-G6</f>
-        <v>-6.861063464837075E-2</v>
+        <v>-6.86106346483705E-2</v>
       </c>
       <c r="H22" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>-3.7364341085271313E-2</v>
+        <v>1.6169942929613185E-2</v>
       </c>
       <c r="I22" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>-3.5653070303329398E-2</v>
+        <v>9.107253170153512E-3</v>
       </c>
       <c r="K22" s="2">
         <f ca="1">H6*$D$8*F22</f>
-        <v>-1000000.0000000036</v>
+        <v>-720000.00000000012</v>
       </c>
       <c r="L22" s="3">
         <f t="shared" ca="1" si="16"/>
-        <v>-321333.33333333378</v>
+        <v>122891.5662650602</v>
       </c>
       <c r="M22" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>-319767.44186046562</v>
+        <v>165789.47368421053</v>
       </c>
       <c r="N22" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>-1641100.775193803</v>
+        <v>-431318.96005072934</v>
       </c>
       <c r="O22" s="3">
         <f t="shared" ca="1" si="11"/>
-        <v>-281100.77519379929</v>
+        <v>108681.03994927066</v>
       </c>
       <c r="P22" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>0.20669174646602831</v>
+        <v>-0.20126118509124197</v>
       </c>
       <c r="R22" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>1000000.0000000036</v>
+        <v>720000.00000000012</v>
       </c>
       <c r="S22" s="3">
         <f t="shared" ca="1" si="20"/>
-        <v>133017.05426356607</v>
+        <v>-51840.83703233987</v>
       </c>
       <c r="T22" s="3">
         <f t="shared" ca="1" si="21"/>
-        <v>88953.48837209311</v>
+        <v>-81947.368421052641</v>
       </c>
       <c r="U22" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>1221970.5426356627</v>
+        <v>586211.79454660765</v>
       </c>
       <c r="V22" s="3">
         <f t="shared" ca="1" si="23"/>
-        <v>-138029.45736434101</v>
+        <v>46211.794546607649</v>
       </c>
       <c r="W22" s="5">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.10149224806201518</v>
+        <v>8.5577397308532685E-2</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -23315,83 +23310,83 @@
       </c>
       <c r="B23" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>-1069999.9999999998</v>
+        <v>30000</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>-930000.00000000023</v>
+        <v>-30000</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" ref="D23" ca="1" si="29">D15-D7</f>
-        <v>-2000000</v>
+        <v>0</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>-139999.99999999953</v>
+        <v>60000</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" ca="1" si="8"/>
-        <v>2.0000000000000157E-2</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="G23" s="5">
         <f ca="1">G15-G7</f>
-        <v>3.24675324675327E-2</v>
+        <v>3.2467532467532451E-2</v>
       </c>
       <c r="H23" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>-1.8139534883720929E-2</v>
+        <v>-3.3291058972733031E-3</v>
       </c>
       <c r="I23" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>-1.4996841097877363E-2</v>
+        <v>-2.1678868979258317E-3</v>
       </c>
       <c r="K23" s="2">
         <f ca="1">H7*$D$8*F23</f>
-        <v>100000.00000000079</v>
+        <v>60000.000000000015</v>
       </c>
       <c r="L23" s="3">
         <f t="shared" ca="1" si="16"/>
-        <v>-156000</v>
+        <v>-25301.204819277144</v>
       </c>
       <c r="M23" s="3">
         <f t="shared" ca="1" si="17"/>
-        <v>-63953.488372093023</v>
+        <v>27631.578947368464</v>
       </c>
       <c r="N23" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>-119953.48837209224</v>
+        <v>62330.374128091331</v>
       </c>
       <c r="O23" s="3">
         <f t="shared" ca="1" si="11"/>
-        <v>20046.511627907297</v>
+        <v>2330.3741280913309</v>
       </c>
       <c r="P23" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>-0.14318936877076688</v>
+        <v>3.883956880152218E-2</v>
       </c>
       <c r="R23" s="2">
         <f t="shared" ca="1" si="19"/>
-        <v>-100000.00000000079</v>
+        <v>-60000.000000000015</v>
       </c>
       <c r="S23" s="3">
         <f t="shared" ca="1" si="20"/>
-        <v>64576.744186046504</v>
+        <v>10673.113506658226</v>
       </c>
       <c r="T23" s="3">
         <f t="shared" ca="1" si="21"/>
-        <v>17790.697674418592</v>
+        <v>-13657.894736842127</v>
       </c>
       <c r="U23" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>-17632.558139535689</v>
+        <v>-62984.781230183915</v>
       </c>
       <c r="V23" s="3">
         <f t="shared" ca="1" si="23"/>
-        <v>-157632.55813953522</v>
+        <v>-2984.7812301839149</v>
       </c>
       <c r="W23" s="5">
         <f t="shared" ca="1" si="24"/>
-        <v>-1.1259468438538267</v>
+        <v>4.9746353836398582E-2</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
@@ -23400,27 +23395,27 @@
       </c>
       <c r="B24" s="3">
         <f ca="1">SUM(B19:B23)</f>
-        <v>-7940000.0000000019</v>
+        <v>3540000</v>
       </c>
       <c r="C24" s="3">
         <f ca="1">SUM(C19:C23)</f>
-        <v>-3059999.9999999981</v>
+        <v>3460000</v>
       </c>
       <c r="D24" s="3">
         <f ca="1">SUM(D19:D23)</f>
-        <v>-11000000</v>
+        <v>7000000</v>
       </c>
       <c r="E24" s="3">
         <f ca="1">SUM(E19:E23)</f>
-        <v>-4880000.0000000037</v>
+        <v>80000</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" ca="1" si="8"/>
-        <v>-3.9826356589147321E-2</v>
+        <v>-1.2219403931515549E-2</v>
       </c>
       <c r="G24" s="5">
         <f t="shared" ref="G24" ca="1" si="30">G16-G8</f>
-        <v>-6.0019140330021231E-2</v>
+        <v>-1.8473149607778738E-2</v>
       </c>
       <c r="H24" s="5">
         <f t="shared" ca="1" si="10"/>
@@ -23432,51 +23427,51 @@
       </c>
       <c r="K24" s="3">
         <f ca="1">SUM(K19:K23)</f>
-        <v>-2480000.0000000047</v>
+        <v>-1880000.0000000005</v>
       </c>
       <c r="L24" s="3">
         <f ca="1">SUM(L19:L23)</f>
-        <v>-1246400.0000000007</v>
+        <v>1232289.156626506</v>
       </c>
       <c r="M24" s="3">
         <f ca="1">SUM(M19:M23)</f>
-        <v>-1893023.2558139542</v>
+        <v>1094210.5263157894</v>
       </c>
       <c r="N24" s="3">
         <f t="shared" ca="1" si="18"/>
-        <v>-5619423.25581396</v>
+        <v>446499.68294229498</v>
       </c>
       <c r="O24" s="3">
         <f t="shared" ca="1" si="11"/>
-        <v>-739423.25581395626</v>
+        <v>366499.68294229498</v>
       </c>
       <c r="P24" s="5">
         <f t="shared" ca="1" si="12"/>
-        <v>0.15152115897826962</v>
+        <v>4.5812460367786869</v>
       </c>
       <c r="R24" s="3">
         <f ca="1">SUM(R19:R23)</f>
-        <v>2480000.0000000047</v>
+        <v>1880000.0000000005</v>
       </c>
       <c r="S24" s="3">
         <f ca="1">SUM(S19:S23)</f>
-        <v>515951.62790697697</v>
+        <v>-519831.45212428668</v>
       </c>
       <c r="T24" s="3">
         <f ca="1">SUM(T19:T23)</f>
-        <v>526604.6511627906</v>
+        <v>-540852.6315789473</v>
       </c>
       <c r="U24" s="3">
         <f t="shared" ca="1" si="22"/>
-        <v>3522556.2790697725</v>
+        <v>819315.91629676649</v>
       </c>
       <c r="V24" s="3">
         <f t="shared" ca="1" si="23"/>
-        <v>-1357443.7209302313</v>
+        <v>899315.91629676649</v>
       </c>
       <c r="W24" s="5">
         <f t="shared" ca="1" si="24"/>
-        <v>-0.27816469691193241</v>
+        <v>-11.241448953709581</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
@@ -23521,11 +23516,11 @@
       </c>
       <c r="H27" s="5">
         <f ca="1">H3</f>
-        <v>0.13953488372093023</v>
+        <v>0.13157894736842105</v>
       </c>
       <c r="I27" s="5">
         <f ca="1">C3/C8</f>
-        <v>1.6853932584269663E-3</v>
+        <v>1.5595757953836558E-3</v>
       </c>
       <c r="K27" t="s">
         <v>16</v>
@@ -23576,59 +23571,59 @@
       </c>
       <c r="H28" s="5">
         <f t="shared" ref="H28:H32" ca="1" si="33">H4</f>
-        <v>0.43023255813953487</v>
+        <v>0.5</v>
       </c>
       <c r="I28" s="5">
         <f ca="1">C4/C8</f>
-        <v>0.54044943820224722</v>
+        <v>0.61634435433562074</v>
       </c>
       <c r="K28" s="2">
         <f ca="1">H3*$D$8*F19</f>
-        <v>-2040000.0000000005</v>
+        <v>-1700000.0000000005</v>
       </c>
       <c r="L28" s="3">
         <f ca="1">$D$8*F11*H19</f>
-        <v>-437333.33333333331</v>
+        <v>810120.48192771093</v>
       </c>
       <c r="M28" s="3">
         <f ca="1">F11*H11*$D$24</f>
-        <v>-1202666.6666666665</v>
+        <v>829879.51807228907</v>
       </c>
       <c r="N28" s="3">
         <f ca="1">SUM(K28:M28)</f>
-        <v>-3680000.0000000005</v>
+        <v>-60000.000000000466</v>
       </c>
       <c r="O28" s="3">
         <f t="shared" ref="O28:O33" ca="1" si="34">N28-E19</f>
-        <v>0</v>
+        <v>-4.6566128730773926E-10</v>
       </c>
       <c r="P28" s="1">
         <f t="shared" ref="P28:P33" ca="1" si="35">O28/E19</f>
-        <v>0</v>
+        <v>7.761021455128988E-15</v>
       </c>
       <c r="R28" s="2">
         <f ca="1">H27*$D$8*F43</f>
-        <v>2040000.0000000005</v>
+        <v>1700000.0000000005</v>
       </c>
       <c r="S28" s="3">
         <f ca="1">$D$8*F35*H43</f>
-        <v>437333.33333333331</v>
+        <v>-810120.48192771093</v>
       </c>
       <c r="T28" s="3">
         <f ca="1">F35*H35*$D$24</f>
-        <v>1202666.6666666665</v>
+        <v>-829879.51807228907</v>
       </c>
       <c r="U28" s="3">
         <f ca="1">SUM(R28:T28)</f>
-        <v>3680000.0000000005</v>
+        <v>60000.000000000466</v>
       </c>
       <c r="V28" s="3">
         <f t="shared" ref="V28:V33" ca="1" si="36">U28+E19</f>
-        <v>0</v>
+        <v>4.6566128730773926E-10</v>
       </c>
       <c r="W28" s="1">
         <f t="shared" ref="W28:W33" ca="1" si="37">V28/-E19</f>
-        <v>0</v>
+        <v>7.761021455128988E-15</v>
       </c>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
@@ -23642,23 +23637,23 @@
       </c>
       <c r="H29" s="5">
         <f t="shared" ca="1" si="33"/>
-        <v>8.1395348837209308E-2</v>
+        <v>9.2105263157894732E-2</v>
       </c>
       <c r="I29" s="5">
         <f ca="1">C5/C8</f>
-        <v>7.8651685393258425E-2</v>
+        <v>8.7336244541484712E-2</v>
       </c>
       <c r="K29" s="2">
         <f ca="1">H4*$D$8*F20</f>
-        <v>740000</v>
+        <v>760000</v>
       </c>
       <c r="L29" s="3">
         <f ca="1">$D$8*F12*H20</f>
-        <v>-108533.33333333337</v>
+        <v>45783.132530120463</v>
       </c>
       <c r="M29" s="3">
         <f ca="1">F12*H12*$D$24</f>
-        <v>108533.33333333334</v>
+        <v>-65783.132530120492</v>
       </c>
       <c r="N29" s="3">
         <f t="shared" ref="N29:N33" ca="1" si="38">SUM(K29:M29)</f>
@@ -23674,15 +23669,15 @@
       </c>
       <c r="R29" s="2">
         <f ca="1">H28*$D$8*F44</f>
-        <v>-740000</v>
+        <v>-760000</v>
       </c>
       <c r="S29" s="3">
         <f ca="1">$D$8*F36*H44</f>
-        <v>108533.33333333337</v>
+        <v>-45783.132530120463</v>
       </c>
       <c r="T29" s="3">
         <f ca="1">F36*H36*$D$24</f>
-        <v>-108533.33333333334</v>
+        <v>65783.132530120492</v>
       </c>
       <c r="U29" s="3">
         <f t="shared" ref="U29:U33" ca="1" si="39">SUM(R29:T29)</f>
@@ -23700,35 +23695,35 @@
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F30" s="5">
         <f t="shared" ca="1" si="32"/>
-        <v>-0.10000000000000014</v>
+        <v>-0.1</v>
       </c>
       <c r="G30" s="5">
         <f t="shared" ca="1" si="31"/>
-        <v>-0.2222222222222226</v>
+        <v>-0.22222222222222221</v>
       </c>
       <c r="H30" s="5">
         <f t="shared" ca="1" si="33"/>
-        <v>0.29069767441860467</v>
+        <v>0.23684210526315788</v>
       </c>
       <c r="I30" s="5">
         <f ca="1">C6/C8</f>
-        <v>0.31601123595505615</v>
+        <v>0.25265127885215222</v>
       </c>
       <c r="K30" s="2">
         <f ca="1">H5*$D$8*F21</f>
-        <v>-280000.00000000128</v>
+        <v>-280000.00000000006</v>
       </c>
       <c r="L30" s="3">
         <f ca="1">$D$8*F13*H21</f>
-        <v>-19200.000000000036</v>
+        <v>52048.192771084461</v>
       </c>
       <c r="M30" s="3">
         <f ca="1">F13*H13*$D$24</f>
-        <v>-140799.99999999985</v>
+        <v>107951.80722891567</v>
       </c>
       <c r="N30" s="3">
         <f t="shared" ca="1" si="38"/>
-        <v>-440000.00000000116</v>
+        <v>-119999.99999999993</v>
       </c>
       <c r="O30" s="3">
         <f t="shared" ca="1" si="34"/>
@@ -23740,19 +23735,19 @@
       </c>
       <c r="R30" s="2">
         <f ca="1">H29*$D$8*F45</f>
-        <v>280000.00000000128</v>
+        <v>280000.00000000006</v>
       </c>
       <c r="S30" s="3">
         <f ca="1">$D$8*F37*H45</f>
-        <v>19200.000000000036</v>
+        <v>-52048.192771084461</v>
       </c>
       <c r="T30" s="3">
         <f ca="1">F37*H37*$D$24</f>
-        <v>140799.99999999985</v>
+        <v>-107951.80722891567</v>
       </c>
       <c r="U30" s="3">
         <f t="shared" ca="1" si="39"/>
-        <v>440000.00000000116</v>
+        <v>119999.99999999993</v>
       </c>
       <c r="V30" s="3">
         <f t="shared" ca="1" si="36"/>
@@ -23766,35 +23761,35 @@
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F31" s="5">
         <f t="shared" ca="1" si="32"/>
-        <v>-0.1</v>
+        <v>-0.10000000000000016</v>
       </c>
       <c r="G31" s="5">
         <f t="shared" ca="1" si="31"/>
-        <v>-0.22222222222222221</v>
+        <v>-0.2222222222222226</v>
       </c>
       <c r="H31" s="5">
         <f t="shared" ca="1" si="33"/>
-        <v>5.8139534883720929E-2</v>
+        <v>3.9473684210526314E-2</v>
       </c>
       <c r="I31" s="5">
         <f ca="1">C7/C8</f>
-        <v>6.3202247191011238E-2</v>
+        <v>4.2108546475358694E-2</v>
       </c>
       <c r="K31" s="2">
         <f ca="1">H6*$D$8*F22</f>
-        <v>-1000000.0000000036</v>
+        <v>-720000.00000000012</v>
       </c>
       <c r="L31" s="3">
         <f ca="1">$D$8*F14*H22</f>
-        <v>-192799.99999999997</v>
+        <v>73734.939759036119</v>
       </c>
       <c r="M31" s="3">
         <f ca="1">F14*H14*$D$24</f>
-        <v>-167200</v>
+        <v>106265.06024096385</v>
       </c>
       <c r="N31" s="3">
         <f t="shared" ca="1" si="38"/>
-        <v>-1360000.0000000035</v>
+        <v>-540000.00000000012</v>
       </c>
       <c r="O31" s="3">
         <f t="shared" ca="1" si="34"/>
@@ -23806,19 +23801,19 @@
       </c>
       <c r="R31" s="2">
         <f ca="1">H30*$D$8*F46</f>
-        <v>1000000.0000000036</v>
+        <v>720000.00000000012</v>
       </c>
       <c r="S31" s="3">
         <f ca="1">$D$8*F38*H46</f>
-        <v>192799.99999999997</v>
+        <v>-73734.939759036119</v>
       </c>
       <c r="T31" s="3">
         <f ca="1">F38*H38*$D$24</f>
-        <v>167200</v>
+        <v>-106265.06024096385</v>
       </c>
       <c r="U31" s="3">
         <f t="shared" ca="1" si="39"/>
-        <v>1360000.0000000035</v>
+        <v>540000.00000000012</v>
       </c>
       <c r="V31" s="3">
         <f t="shared" ca="1" si="36"/>
@@ -23832,11 +23827,11 @@
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="F32" s="5">
         <f t="shared" ca="1" si="32"/>
-        <v>-0.17209302325581399</v>
+        <v>-0.15631578947368421</v>
       </c>
       <c r="G32" s="5">
         <f t="shared" ca="1" si="31"/>
-        <v>-0.41573033707865181</v>
+        <v>-0.37055520898315658</v>
       </c>
       <c r="H32" s="5">
         <f t="shared" ca="1" si="33"/>
@@ -23848,19 +23843,19 @@
       </c>
       <c r="K32" s="2">
         <f ca="1">H7*$D$8*F23</f>
-        <v>100000.00000000079</v>
+        <v>60000.000000000015</v>
       </c>
       <c r="L32" s="3">
         <f ca="1">$D$8*F15*H23</f>
-        <v>-187200.00000000023</v>
+        <v>-30361.445783132567</v>
       </c>
       <c r="M32" s="3">
         <f ca="1">F15*H15*$D$24</f>
-        <v>-52800.000000000073</v>
+        <v>30361.445783132567</v>
       </c>
       <c r="N32" s="3">
         <f t="shared" ca="1" si="38"/>
-        <v>-139999.99999999953</v>
+        <v>60000.000000000015</v>
       </c>
       <c r="O32" s="3">
         <f t="shared" ca="1" si="34"/>
@@ -23872,19 +23867,19 @@
       </c>
       <c r="R32" s="2">
         <f ca="1">H31*$D$8*F47</f>
-        <v>-100000.00000000079</v>
+        <v>-60000.000000000015</v>
       </c>
       <c r="S32" s="3">
         <f ca="1">$D$8*F39*H47</f>
-        <v>187200.00000000023</v>
+        <v>30361.445783132567</v>
       </c>
       <c r="T32" s="3">
         <f ca="1">F39*H39*$D$24</f>
-        <v>52800.000000000073</v>
+        <v>-30361.445783132567</v>
       </c>
       <c r="U32" s="3">
         <f t="shared" ca="1" si="39"/>
-        <v>139999.99999999953</v>
+        <v>-60000.000000000015</v>
       </c>
       <c r="V32" s="3">
         <f t="shared" ca="1" si="36"/>
@@ -23899,51 +23894,51 @@
       <c r="G33" s="5"/>
       <c r="K33" s="3">
         <f ca="1">SUM(K28:K32)</f>
-        <v>-2480000.0000000047</v>
+        <v>-1880000.0000000005</v>
       </c>
       <c r="L33" s="3">
         <f ca="1">SUM(L28:L32)</f>
-        <v>-945066.66666666698</v>
+        <v>951325.30120481935</v>
       </c>
       <c r="M33" s="3">
         <f ca="1">SUM(M28:M32)</f>
-        <v>-1454933.333333333</v>
+        <v>1008674.6987951805</v>
       </c>
       <c r="N33" s="3">
         <f t="shared" ca="1" si="38"/>
-        <v>-4880000.0000000047</v>
+        <v>79999.999999999418</v>
       </c>
       <c r="O33" s="3">
         <f t="shared" ca="1" si="34"/>
-        <v>0</v>
+        <v>-5.8207660913467407E-10</v>
       </c>
       <c r="P33" s="1">
         <f t="shared" ca="1" si="35"/>
-        <v>0</v>
+        <v>-7.2759576141834261E-15</v>
       </c>
       <c r="R33" s="3">
         <f ca="1">SUM(R28:R32)</f>
-        <v>2480000.0000000047</v>
+        <v>1880000.0000000005</v>
       </c>
       <c r="S33" s="3">
         <f ca="1">SUM(S28:S32)</f>
-        <v>945066.66666666698</v>
+        <v>-951325.30120481935</v>
       </c>
       <c r="T33" s="3">
         <f ca="1">SUM(T28:T32)</f>
-        <v>1454933.333333333</v>
+        <v>-1008674.6987951805</v>
       </c>
       <c r="U33" s="3">
         <f t="shared" ca="1" si="39"/>
-        <v>4880000.0000000047</v>
+        <v>-79999.999999999418</v>
       </c>
       <c r="V33" s="3">
         <f t="shared" ca="1" si="36"/>
-        <v>0</v>
+        <v>5.8207660913467407E-10</v>
       </c>
       <c r="W33" s="1">
         <f t="shared" ca="1" si="37"/>
-        <v>0</v>
+        <v>-7.2759576141834261E-15</v>
       </c>
     </row>
     <row r="34" spans="6:23" x14ac:dyDescent="0.25">
@@ -23971,11 +23966,11 @@
       </c>
       <c r="H35" s="5">
         <f t="shared" ref="H35:H40" ca="1" si="41">H11</f>
-        <v>0.13333333333333333</v>
+        <v>0.14457831325301204</v>
       </c>
       <c r="I35" s="5">
         <f ca="1">C11/C16</f>
-        <v>2.7658266748617086E-2</v>
+        <v>3.0405405405405407E-2</v>
       </c>
       <c r="K35" s="50" t="s">
         <v>31</v>
@@ -24005,11 +24000,11 @@
       </c>
       <c r="H36" s="5">
         <f t="shared" ca="1" si="41"/>
-        <v>0.49333333333333335</v>
+        <v>0.46987951807228917</v>
       </c>
       <c r="I36" s="5">
         <f ca="1">C12/C16</f>
-        <v>0.57990165949600492</v>
+        <v>0.55996621621621623</v>
       </c>
       <c r="K36" t="s">
         <v>16</v>
@@ -24051,67 +24046,67 @@
     <row r="37" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F37" s="5">
         <f t="shared" ca="1" si="42"/>
-        <v>-0.15999999999999984</v>
+        <v>-0.16</v>
       </c>
       <c r="G37" s="5">
         <f t="shared" ca="1" si="40"/>
-        <v>-0.38095238095238049</v>
+        <v>-0.38095238095238093</v>
       </c>
       <c r="H37" s="5">
         <f t="shared" ca="1" si="41"/>
-        <v>0.08</v>
+        <v>9.6385542168674704E-2</v>
       </c>
       <c r="I37" s="5">
         <f ca="1">C13/C16</f>
-        <v>7.7443146896127857E-2</v>
+        <v>9.45945945945946E-2</v>
       </c>
       <c r="K37" s="2">
         <f ca="1">I3*$B$8*G19</f>
-        <v>-1120879.1208791204</v>
+        <v>-934065.93406593369</v>
       </c>
       <c r="L37" s="3">
         <f ca="1">$B$8*G11*I19</f>
-        <v>-1025724.7415796634</v>
+        <v>140418.0823388907</v>
       </c>
       <c r="M37" s="3">
         <f ca="1">G11*I11*$B$24</f>
-        <v>-1533396.1375412156</v>
+        <v>733647.85172704293</v>
       </c>
       <c r="N37" s="3">
         <f ca="1">SUM(K37:M37)</f>
-        <v>-3679999.9999999991</v>
+        <v>-60000.000000000116</v>
       </c>
       <c r="O37" s="3">
         <f t="shared" ref="O37:O42" ca="1" si="43">N37-E19</f>
-        <v>0</v>
+        <v>-1.1641532182693481E-10</v>
       </c>
       <c r="P37" s="1">
         <f t="shared" ref="P37:P42" ca="1" si="44">O37/E19</f>
-        <v>0</v>
+        <v>1.940255363782247E-15</v>
       </c>
       <c r="R37" s="2">
         <f ca="1">I27*$C$8*G43</f>
-        <v>11333333.333333334</v>
+        <v>9444444.444444444</v>
       </c>
       <c r="S37" s="3">
         <f ca="1">$C$8*G35*I43</f>
-        <v>-8424445.8102847766</v>
+        <v>-8425930.9309309311</v>
       </c>
       <c r="T37" s="3">
         <f ca="1">G35*I35*$C$24</f>
-        <v>771112.47695144382</v>
+        <v>-958513.51351351349</v>
       </c>
       <c r="U37" s="3">
         <f ca="1">SUM(R37:T37)</f>
-        <v>3680000.0000000009</v>
+        <v>59999.999999999418</v>
       </c>
       <c r="V37" s="3">
         <f t="shared" ref="V37:V42" ca="1" si="45">U37+E19</f>
-        <v>0</v>
+        <v>-5.8207660913467407E-10</v>
       </c>
       <c r="W37" s="1">
         <f t="shared" ref="W37:W42" ca="1" si="46">V37/-E19</f>
-        <v>0</v>
+        <v>-9.7012768189112342E-15</v>
       </c>
     </row>
     <row r="38" spans="6:23" x14ac:dyDescent="0.25">
@@ -24125,23 +24120,23 @@
       </c>
       <c r="H38" s="5">
         <f t="shared" ca="1" si="41"/>
-        <v>0.25333333333333335</v>
+        <v>0.25301204819277107</v>
       </c>
       <c r="I38" s="5">
         <f ca="1">C14/C16</f>
-        <v>0.2744314689612784</v>
+        <v>0.2778716216216216</v>
       </c>
       <c r="K38" s="2">
         <f ca="1">I4*$B$8*G20</f>
-        <v>755102.04081632651</v>
+        <v>775510.20408163266</v>
       </c>
       <c r="L38" s="3">
         <f ca="1">$B$8*G12*I20</f>
-        <v>-153481.69225297272</v>
+        <v>22644.808555267107</v>
       </c>
       <c r="M38" s="3">
         <f ca="1">G12*I12*$B$24</f>
-        <v>138379.65143664629</v>
+        <v>-58155.012636899744</v>
       </c>
       <c r="N38" s="3">
         <f t="shared" ref="N38:N42" ca="1" si="47">SUM(K38:M38)</f>
@@ -24157,19 +24152,19 @@
       </c>
       <c r="R38" s="2">
         <f ca="1">I28*$C$8*G44</f>
-        <v>-725490.19607843144</v>
+        <v>-745098.03921568638</v>
       </c>
       <c r="S38" s="3">
         <f ca="1">$C$8*G36*I44</f>
-        <v>55078.395217951911</v>
+        <v>-70881.690514043468</v>
       </c>
       <c r="T38" s="3">
         <f ca="1">G36*I36*$C$24</f>
-        <v>-69588.19913952054</v>
+        <v>75979.729729729734</v>
       </c>
       <c r="U38" s="3">
         <f t="shared" ref="U38:U42" ca="1" si="48">SUM(R38:T38)</f>
-        <v>-740000</v>
+        <v>-740000.00000000012</v>
       </c>
       <c r="V38" s="3">
         <f t="shared" ca="1" si="45"/>
@@ -24191,51 +24186,51 @@
       </c>
       <c r="H39" s="5">
         <f t="shared" ca="1" si="41"/>
-        <v>0.04</v>
+        <v>3.614457831325301E-2</v>
       </c>
       <c r="I39" s="5">
         <f ca="1">C15/C16</f>
-        <v>4.0565457897971717E-2</v>
+        <v>3.7162162162162157E-2</v>
       </c>
       <c r="K39" s="2">
         <f ca="1">I5*$B$8*G21</f>
-        <v>-241379.31034482847</v>
+        <v>-241379.31034482754</v>
       </c>
       <c r="L39" s="3">
         <f ca="1">$B$8*G13*I21</f>
-        <v>-19101.14184546921</v>
+        <v>25945.443453505057</v>
       </c>
       <c r="M39" s="3">
         <f ca="1">G13*I13*$B$24</f>
-        <v>-179519.54780970313</v>
+        <v>95433.866891322672</v>
       </c>
       <c r="N39" s="3">
         <f t="shared" ca="1" si="47"/>
-        <v>-440000.00000000081</v>
+        <v>-119999.99999999981</v>
       </c>
       <c r="O39" s="3">
         <f t="shared" ca="1" si="43"/>
-        <v>0</v>
+        <v>1.8917489796876907E-10</v>
       </c>
       <c r="P39" s="1">
         <f t="shared" ca="1" si="44"/>
-        <v>0</v>
+        <v>-1.5764574830730755E-15</v>
       </c>
       <c r="R39" s="2">
         <f ca="1">I29*$C$8*G45</f>
-        <v>333333.33333333465</v>
+        <v>333333.33333333337</v>
       </c>
       <c r="S39" s="3">
         <f ca="1">$C$8*G37*I45</f>
-        <v>16390.083999180253</v>
+        <v>-88648.648648648756</v>
       </c>
       <c r="T39" s="3">
         <f ca="1">G37*I37*$C$24</f>
-        <v>90276.582667486015</v>
+        <v>-124684.68468468469</v>
       </c>
       <c r="U39" s="3">
         <f t="shared" ca="1" si="48"/>
-        <v>440000.00000000093</v>
+        <v>119999.99999999993</v>
       </c>
       <c r="V39" s="3">
         <f t="shared" ca="1" si="45"/>
@@ -24249,11 +24244,11 @@
     <row r="40" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F40" s="5">
         <f t="shared" ca="1" si="42"/>
-        <v>-0.13226666666666667</v>
+        <v>-0.14409638554216866</v>
       </c>
       <c r="G40" s="5">
         <f t="shared" ca="1" si="40"/>
-        <v>-0.30485556238475719</v>
+        <v>-0.33671171171171171</v>
       </c>
       <c r="H40" s="5">
         <f t="shared" ca="1" si="41"/>
@@ -24265,19 +24260,19 @@
       </c>
       <c r="K40" s="2">
         <f ca="1">I6*$B$8*G22</f>
-        <v>-943396.22641509795</v>
+        <v>-679245.28301886795</v>
       </c>
       <c r="L40" s="3">
         <f ca="1">$B$8*G14*I22</f>
-        <v>-203424.3105608832</v>
+        <v>45302.570297722108</v>
       </c>
       <c r="M40" s="3">
         <f ca="1">G14*I14*$B$24</f>
-        <v>-213179.46302402267</v>
+        <v>93942.712721145741</v>
       </c>
       <c r="N40" s="3">
         <f t="shared" ca="1" si="47"/>
-        <v>-1360000.000000004</v>
+        <v>-540000.00000000012</v>
       </c>
       <c r="O40" s="3">
         <f t="shared" ca="1" si="43"/>
@@ -24289,19 +24284,19 @@
       </c>
       <c r="R40" s="2">
         <f ca="1">I30*$C$8*G46</f>
-        <v>1063829.7872340467</v>
+        <v>765957.44680851058</v>
       </c>
       <c r="S40" s="3">
         <f ca="1">$C$8*G38*I46</f>
-        <v>188966.7708483176</v>
+        <v>-103220.96032202404</v>
       </c>
       <c r="T40" s="3">
         <f ca="1">G38*I38*$C$24</f>
-        <v>107203.44191763974</v>
+        <v>-122736.48648648645</v>
       </c>
       <c r="U40" s="3">
         <f t="shared" ca="1" si="48"/>
-        <v>1360000.000000004</v>
+        <v>540000</v>
       </c>
       <c r="V40" s="3">
         <f t="shared" ca="1" si="45"/>
@@ -24315,19 +24310,19 @@
     <row r="41" spans="6:23" x14ac:dyDescent="0.25">
       <c r="K41" s="2">
         <f ca="1">I7*$B$8*G23</f>
-        <v>89285.71428571493</v>
+        <v>53571.428571428551</v>
       </c>
       <c r="L41" s="3">
         <f ca="1">$B$8*G15*I23</f>
-        <v>-161965.88385707568</v>
+        <v>-20412.203634613106</v>
       </c>
       <c r="M41" s="3">
         <f ca="1">G15*I15*$B$24</f>
-        <v>-67319.830428638816</v>
+        <v>26840.775063184534</v>
       </c>
       <c r="N41" s="3">
         <f t="shared" ca="1" si="47"/>
-        <v>-139999.99999999956</v>
+        <v>59999.999999999978</v>
       </c>
       <c r="O41" s="3">
         <f t="shared" ca="1" si="43"/>
@@ -24339,27 +24334,27 @@
       </c>
       <c r="R41" s="2">
         <f ca="1">I31*$C$8*G47</f>
-        <v>-113636.36363636462</v>
+        <v>-68181.818181818235</v>
       </c>
       <c r="S41" s="3">
         <f ca="1">$C$8*G39*I47</f>
-        <v>219782.64513605679</v>
+        <v>43249.385749385779</v>
       </c>
       <c r="T41" s="3">
         <f ca="1">G39*I39*$C$24</f>
-        <v>33853.718500307339</v>
+        <v>-35067.567567567618</v>
       </c>
       <c r="U41" s="3">
         <f t="shared" ca="1" si="48"/>
-        <v>139999.99999999951</v>
+        <v>-60000.000000000073</v>
       </c>
       <c r="V41" s="3">
         <f t="shared" ca="1" si="45"/>
-        <v>0</v>
+        <v>-7.2759576141834259E-11</v>
       </c>
       <c r="W41" s="1">
         <f t="shared" ca="1" si="46"/>
-        <v>0</v>
+        <v>1.2126596023639043E-15</v>
       </c>
     </row>
     <row r="42" spans="6:23" x14ac:dyDescent="0.25">
@@ -24377,51 +24372,51 @@
       </c>
       <c r="K42" s="3">
         <f ca="1">SUM(K37:K41)</f>
-        <v>-1461266.9025370053</v>
+        <v>-1025608.8947765679</v>
       </c>
       <c r="L42" s="3">
         <f ca="1">SUM(L37:L41)</f>
-        <v>-1563697.7700960641</v>
+        <v>213898.70101077188</v>
       </c>
       <c r="M42" s="3">
         <f ca="1">SUM(M37:M41)</f>
-        <v>-1855035.3273669339</v>
+        <v>891710.19376579614</v>
       </c>
       <c r="N42" s="3">
         <f t="shared" ca="1" si="47"/>
-        <v>-4880000.0000000037</v>
+        <v>80000.000000000116</v>
       </c>
       <c r="O42" s="3">
         <f t="shared" ca="1" si="43"/>
-        <v>0</v>
+        <v>1.1641532182693481E-10</v>
       </c>
       <c r="P42" s="1">
         <f t="shared" ca="1" si="44"/>
-        <v>0</v>
+        <v>1.4551915228366853E-15</v>
       </c>
       <c r="R42" s="3">
         <f ca="1">SUM(R37:R41)</f>
-        <v>11891369.894185919</v>
+        <v>9730455.3671887852</v>
       </c>
       <c r="S42" s="3">
         <f ca="1">SUM(S37:S41)</f>
-        <v>-7944227.9150832696</v>
+        <v>-8645432.8446662612</v>
       </c>
       <c r="T42" s="3">
         <f ca="1">SUM(T37:T41)</f>
-        <v>932858.02089735633</v>
+        <v>-1165022.5225225226</v>
       </c>
       <c r="U42" s="3">
         <f t="shared" ca="1" si="48"/>
-        <v>4880000.0000000056</v>
+        <v>-79999.999999998603</v>
       </c>
       <c r="V42" s="3">
         <f t="shared" ca="1" si="45"/>
-        <v>0</v>
+        <v>1.3969838619232178E-9</v>
       </c>
       <c r="W42" s="1">
         <f t="shared" ca="1" si="46"/>
-        <v>0</v>
+        <v>-1.7462298274040221E-14</v>
       </c>
     </row>
     <row r="43" spans="6:23" x14ac:dyDescent="0.25">
@@ -24435,11 +24430,11 @@
       </c>
       <c r="H43" s="5">
         <f t="shared" ca="1" si="50"/>
-        <v>-6.2015503875968991E-3</v>
+        <v>1.2999365884590997E-2</v>
       </c>
       <c r="I43" s="5">
         <f t="shared" ref="I43" ca="1" si="51">I35-I27</f>
-        <v>2.5972873490190118E-2</v>
+        <v>2.8845829610021752E-2</v>
       </c>
     </row>
     <row r="44" spans="6:23" x14ac:dyDescent="0.25">
@@ -24453,75 +24448,75 @@
       </c>
       <c r="H44" s="5">
         <f t="shared" ca="1" si="50"/>
-        <v>6.3100775193798475E-2</v>
+        <v>-3.0120481927710829E-2</v>
       </c>
       <c r="I44" s="5">
         <f t="shared" ref="I44" ca="1" si="53">I36-I28</f>
-        <v>3.9452221293757694E-2</v>
+        <v>-5.6378138119404508E-2</v>
       </c>
     </row>
     <row r="45" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F45" s="5">
         <f t="shared" ref="F45" ca="1" si="54">F37-F29</f>
-        <v>4.0000000000000174E-2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="G45" s="5">
         <f t="shared" ca="1" si="50"/>
-        <v>0.11904761904761951</v>
+        <v>0.11904761904761907</v>
       </c>
       <c r="H45" s="5">
         <f t="shared" ca="1" si="50"/>
-        <v>-1.3953488372093065E-3</v>
+        <v>4.2802790107799721E-3</v>
       </c>
       <c r="I45" s="5">
         <f t="shared" ref="I45" ca="1" si="55">I37-I29</f>
-        <v>-1.2085384971305679E-3</v>
+        <v>7.2583500531098882E-3</v>
       </c>
     </row>
     <row r="46" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F46" s="5">
         <f t="shared" ref="F46" ca="1" si="56">F38-F30</f>
-        <v>4.0000000000000147E-2</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="G46" s="5">
         <f t="shared" ca="1" si="50"/>
-        <v>9.4562647754137502E-2</v>
+        <v>9.4562647754137114E-2</v>
       </c>
       <c r="H46" s="5">
         <f t="shared" ca="1" si="50"/>
-        <v>-3.7364341085271313E-2</v>
+        <v>1.6169942929613185E-2</v>
       </c>
       <c r="I46" s="5">
         <f t="shared" ref="I46" ca="1" si="57">I38-I30</f>
-        <v>-4.1579766993777745E-2</v>
+        <v>2.5220342769469384E-2</v>
       </c>
     </row>
     <row r="47" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F47" s="5">
         <f t="shared" ref="F47" ca="1" si="58">F39-F31</f>
-        <v>-2.0000000000000157E-2</v>
+        <v>-2.0000000000000004E-2</v>
       </c>
       <c r="G47" s="5">
         <f t="shared" ca="1" si="50"/>
-        <v>-5.0505050505050941E-2</v>
+        <v>-5.0505050505050553E-2</v>
       </c>
       <c r="H47" s="5">
         <f t="shared" ca="1" si="50"/>
-        <v>-1.8139534883720929E-2</v>
+        <v>-3.3291058972733031E-3</v>
       </c>
       <c r="I47" s="5">
         <f t="shared" ref="I47" ca="1" si="59">I39-I31</f>
-        <v>-2.2636789293039521E-2</v>
+        <v>-4.9463843131965363E-3</v>
       </c>
     </row>
     <row r="48" spans="6:23" x14ac:dyDescent="0.25">
       <c r="F48" s="5">
         <f t="shared" ref="F48" ca="1" si="60">F40-F32</f>
-        <v>3.9826356589147321E-2</v>
+        <v>1.2219403931515549E-2</v>
       </c>
       <c r="G48" s="5">
         <f t="shared" ca="1" si="50"/>
-        <v>0.11087477469389462</v>
+        <v>3.3843497271444867E-2</v>
       </c>
       <c r="H48" s="5">
         <f t="shared" ca="1" si="50"/>
@@ -29407,8 +29402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8BA39E4-3417-46FF-A4A1-9CD6CACB2BC8}">
   <dimension ref="A1:Y62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31827,8 +31822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCEA7996-F24A-4990-8704-B7838C34375B}">
   <dimension ref="A1:Y62"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31924,23 +31919,23 @@
       </c>
       <c r="B3" s="2">
         <f>I3*J3</f>
-        <v>15568444.444444446</v>
+        <v>15896319.768888889</v>
       </c>
       <c r="C3" s="2">
         <f>J3-B3</f>
-        <v>1353777.777777778</v>
+        <v>1382288.6755555551</v>
       </c>
       <c r="D3" s="2">
         <f>SUM(B3:C3)</f>
-        <v>16922222.222222224</v>
+        <v>17278608.444444444</v>
       </c>
       <c r="E3" s="2">
         <f>B3-C3</f>
-        <v>14214666.666666668</v>
+        <v>14514031.093333334</v>
       </c>
       <c r="F3" s="10">
         <f>E3/D3</f>
-        <v>0.84</v>
+        <v>0.84000000000000008</v>
       </c>
       <c r="G3" s="10">
         <f>D3/D$8</f>
@@ -31951,8 +31946,8 @@
         <v>0.92</v>
       </c>
       <c r="J3" s="6">
-        <f>K3*$V$11</f>
-        <v>16922222.222222224</v>
+        <f>K3*$V$3</f>
+        <v>17278608.444444444</v>
       </c>
       <c r="K3" s="5">
         <f>1/$N$16*N3</f>
@@ -31968,8 +31963,7 @@
         <v>0.11</v>
       </c>
       <c r="V3" s="2">
-        <f>74000000+81000000</f>
-        <v>155000000</v>
+        <v>155507476</v>
       </c>
       <c r="X3" s="10"/>
       <c r="Y3" s="11"/>
@@ -31980,35 +31974,35 @@
       </c>
       <c r="B4" s="2">
         <f t="shared" ref="B4:B7" si="0">I4*J4</f>
-        <v>9674372.5918983668</v>
+        <v>9878117.2925127596</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" ref="C4:C7" si="1">J4-B4</f>
-        <v>5709465.7919400185</v>
+        <v>5829708.566073101</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" ref="D4:D7" si="2">SUM(B4:C4)</f>
-        <v>15383838.383838385</v>
+        <v>15707825.858585861</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" ref="E4:E7" si="3">B4-C4</f>
-        <v>3964906.7999583483</v>
+        <v>4048408.7264396586</v>
       </c>
       <c r="F4" s="10">
         <f t="shared" ref="F4:F8" si="4">E4/D4</f>
-        <v>0.25773195876288668</v>
+        <v>0.25773195876288685</v>
       </c>
       <c r="G4" s="10">
         <f>D4/D$8</f>
-        <v>0.1</v>
+        <v>0.10000000000000002</v>
       </c>
       <c r="I4" s="7">
         <f t="shared" ref="I4:I7" si="5">(1/(L4+M4))*L4</f>
         <v>0.6288659793814434</v>
       </c>
       <c r="J4" s="6">
-        <f t="shared" ref="J4:J7" si="6">K4*$V$11</f>
-        <v>15383838.383838385</v>
+        <f t="shared" ref="J4:J7" si="6">K4*$V$3</f>
+        <v>15707825.858585861</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" ref="K4:K7" si="7">1/$N$16*N4</f>
@@ -32032,27 +32026,27 @@
       </c>
       <c r="B5" s="2">
         <f t="shared" si="0"/>
-        <v>4307474.7474747477</v>
+        <v>4398191.2404040406</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" si="1"/>
-        <v>1846060.6060606064</v>
+        <v>1884939.1030303035</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ref="D5" si="8">SUM(B5:C5)</f>
-        <v>6153535.3535353541</v>
+        <v>6283130.343434344</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="3"/>
-        <v>2461414.1414141413</v>
+        <v>2513252.1373737371</v>
       </c>
       <c r="F5" s="10">
         <f t="shared" si="4"/>
-        <v>0.39999999999999997</v>
+        <v>0.39999999999999991</v>
       </c>
       <c r="G5" s="10">
         <f t="shared" ref="G5" si="9">D5/D$8</f>
-        <v>0.04</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="5"/>
@@ -32060,7 +32054,7 @@
       </c>
       <c r="J5" s="6">
         <f t="shared" si="6"/>
-        <v>6153535.3535353541</v>
+        <v>6283130.343434344</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="7"/>
@@ -32084,27 +32078,27 @@
       </c>
       <c r="B6" s="2">
         <f t="shared" si="0"/>
-        <v>1794781.1447811448</v>
+        <v>1832579.6835016834</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" si="1"/>
-        <v>1281986.5319865323</v>
+        <v>1308985.4882154886</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="2"/>
-        <v>3076767.6767676771</v>
+        <v>3141565.171717172</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="3"/>
-        <v>512794.61279461253</v>
+        <v>523594.19528619479</v>
       </c>
       <c r="F6" s="10">
         <f t="shared" si="4"/>
-        <v>0.16666666666666657</v>
+        <v>0.16666666666666649</v>
       </c>
       <c r="G6" s="10">
         <f>D6/D$8</f>
-        <v>0.02</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="I6" s="7">
         <f t="shared" si="5"/>
@@ -32112,7 +32106,7 @@
       </c>
       <c r="J6" s="6">
         <f t="shared" si="6"/>
-        <v>3076767.6767676771</v>
+        <v>3141565.171717172</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="7"/>
@@ -32135,19 +32129,19 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" si="0"/>
-        <v>49275376.21109049</v>
+        <v>50313127.928674497</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" si="1"/>
-        <v>63026643.990929708</v>
+        <v>64354000.839002274</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="2"/>
-        <v>112302020.2020202</v>
+        <v>114667128.76767677</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="3"/>
-        <v>-13751267.779839218</v>
+        <v>-14040872.910327777</v>
       </c>
       <c r="F7" s="10">
         <f t="shared" si="4"/>
@@ -32155,7 +32149,7 @@
       </c>
       <c r="G7" s="10">
         <f>D7/D$8</f>
-        <v>0.72999999999999987</v>
+        <v>0.73</v>
       </c>
       <c r="I7" s="7">
         <f t="shared" si="5"/>
@@ -32163,7 +32157,7 @@
       </c>
       <c r="J7" s="6">
         <f t="shared" si="6"/>
-        <v>112302020.2020202</v>
+        <v>114667128.76767677</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="7"/>
@@ -32186,23 +32180,23 @@
       </c>
       <c r="B8" s="3">
         <f>SUM(B3:B7)</f>
-        <v>80620449.139689207</v>
+        <v>82318335.91398187</v>
       </c>
       <c r="C8" s="3">
         <f>SUM(C3:C7)</f>
-        <v>73217934.698694646</v>
+        <v>74759922.671876729</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" ref="D8" si="10">SUM(B8:C8)</f>
-        <v>153838383.83838385</v>
+        <v>157078258.58585858</v>
       </c>
       <c r="E8" s="3">
         <f>SUM(E3:E7)</f>
-        <v>7402514.4409945495</v>
+        <v>7558413.2421051487</v>
       </c>
       <c r="F8" s="10">
         <f t="shared" si="4"/>
-        <v>4.8118774107581114E-2</v>
+        <v>4.8118774107581148E-2</v>
       </c>
       <c r="G8" s="10">
         <f>D8/D$8</f>
@@ -32269,19 +32263,19 @@
       </c>
       <c r="B11" s="2">
         <f>I11*J11</f>
-        <v>14700112.233445568</v>
+        <v>14702061.277216613</v>
       </c>
       <c r="C11" s="2">
         <f>J11-B11</f>
-        <v>2222109.9887766559</v>
+        <v>2222404.6116722785</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" ref="D11:D16" si="11">SUM(B11:C11)</f>
-        <v>16922222.222222224</v>
+        <v>16924465.888888892</v>
       </c>
       <c r="E11" s="2">
         <f>B11-C11</f>
-        <v>12478002.244668912</v>
+        <v>12479656.665544335</v>
       </c>
       <c r="F11" s="10">
         <f t="shared" ref="F11:F16" si="12">E11/D11</f>
@@ -32289,7 +32283,7 @@
       </c>
       <c r="G11" s="10">
         <f>D11/D$16</f>
-        <v>0.11111111111111112</v>
+        <v>0.11111111111111113</v>
       </c>
       <c r="I11" s="7">
         <f>(1/(L11+M11))*L11</f>
@@ -32297,7 +32291,7 @@
       </c>
       <c r="J11" s="6">
         <f>K11*$V$11</f>
-        <v>16922222.222222224</v>
+        <v>16924465.888888892</v>
       </c>
       <c r="K11" s="5">
         <f>1/$N$16*N11</f>
@@ -32313,8 +32307,7 @@
         <v>0.11</v>
       </c>
       <c r="V11" s="2">
-        <f>77300000+75000000</f>
-        <v>152300000</v>
+        <v>152320193</v>
       </c>
       <c r="X11" s="10"/>
     </row>
@@ -32324,27 +32317,27 @@
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12:B15" si="13">I12*J12</f>
-        <v>8897250.8591065295</v>
+        <v>8898430.518900346</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" ref="C12:C15" si="14">J12-B12</f>
-        <v>8024971.3631156944</v>
+        <v>8026035.3699885458</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" ref="D12:D15" si="15">SUM(B12:C12)</f>
-        <v>16922222.222222224</v>
+        <v>16924465.888888892</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" ref="E12:E15" si="16">B12-C12</f>
-        <v>872279.49599083513</v>
+        <v>872395.14891180024</v>
       </c>
       <c r="F12" s="10">
         <f t="shared" si="12"/>
-        <v>5.1546391752577254E-2</v>
+        <v>5.1546391752577421E-2</v>
       </c>
       <c r="G12" s="10">
         <f>D12/D$16</f>
-        <v>0.11111111111111112</v>
+        <v>0.11111111111111113</v>
       </c>
       <c r="I12" s="7">
         <f t="shared" ref="I12:I15" si="17">(1/(L12+M12))*L12</f>
@@ -32352,7 +32345,7 @@
       </c>
       <c r="J12" s="6">
         <f t="shared" ref="J12:J15" si="18">K12*$V$11</f>
-        <v>16922222.222222224</v>
+        <v>16924465.888888892</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" ref="K12:K15" si="19">1/$N$16*N12</f>
@@ -32375,23 +32368,23 @@
       </c>
       <c r="B13" s="2">
         <f t="shared" si="13"/>
-        <v>2671929.8245614041</v>
+        <v>2672284.0877192984</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="14"/>
-        <v>1943221.6905901115</v>
+        <v>1943479.3365231263</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" ref="D13" si="20">SUM(B13:C13)</f>
-        <v>4615151.5151515156</v>
+        <v>4615763.4242424248</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="16"/>
-        <v>728708.13397129253</v>
+        <v>728804.75119617209</v>
       </c>
       <c r="F13" s="10">
         <f t="shared" si="12"/>
-        <v>0.15789473684210539</v>
+        <v>0.1578947368421052</v>
       </c>
       <c r="G13" s="10">
         <f t="shared" ref="G13" si="21">D13/D$16</f>
@@ -32403,7 +32396,7 @@
       </c>
       <c r="J13" s="6">
         <f t="shared" si="18"/>
-        <v>4615151.5151515156</v>
+        <v>4615763.4242424248</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="19"/>
@@ -32426,23 +32419,23 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" si="13"/>
-        <v>1971054.2929292931</v>
+        <v>1971315.6291035356</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="14"/>
-        <v>2644097.2222222225</v>
+        <v>2644447.795138889</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="15"/>
-        <v>4615151.5151515156</v>
+        <v>4615763.4242424248</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="16"/>
-        <v>-673042.92929292936</v>
+        <v>-673132.16603535344</v>
       </c>
       <c r="F14" s="10">
         <f t="shared" si="12"/>
-        <v>-0.14583333333333334</v>
+        <v>-0.14583333333333329</v>
       </c>
       <c r="G14" s="10">
         <f>D14/D$16</f>
@@ -32454,7 +32447,7 @@
       </c>
       <c r="J14" s="6">
         <f t="shared" si="18"/>
-        <v>4615151.5151515156</v>
+        <v>4615763.4242424248</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="19"/>
@@ -32477,23 +32470,23 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" si="13"/>
-        <v>46337985.919804104</v>
+        <v>46344129.734312825</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="14"/>
-        <v>62887266.605448417</v>
+        <v>62895604.63942454</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="15"/>
-        <v>109225252.52525252</v>
+        <v>109239734.37373737</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="16"/>
-        <v>-16549280.685644314</v>
+        <v>-16551474.905111715</v>
       </c>
       <c r="F15" s="10">
         <f t="shared" si="12"/>
-        <v>-0.15151515151515144</v>
+        <v>-0.15151515151515146</v>
       </c>
       <c r="G15" s="10">
         <f>D15/D$16</f>
@@ -32505,7 +32498,7 @@
       </c>
       <c r="J15" s="6">
         <f t="shared" si="18"/>
-        <v>109225252.52525252</v>
+        <v>109239734.37373737</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="19"/>
@@ -32528,23 +32521,23 @@
       </c>
       <c r="B16" s="3">
         <f>SUM(B11:B15)</f>
-        <v>74578333.129846901</v>
+        <v>74588221.247252613</v>
       </c>
       <c r="C16" s="3">
         <f>SUM(C11:C15)</f>
-        <v>77721666.870153099</v>
+        <v>77731971.752747387</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="11"/>
-        <v>152300000</v>
+        <v>152320193</v>
       </c>
       <c r="E16" s="3">
         <f>SUM(E11:E15)</f>
-        <v>-3143333.7403062023</v>
+        <v>-3143750.5054947622</v>
       </c>
       <c r="F16" s="10">
         <f t="shared" si="12"/>
-        <v>-2.0639092188484587E-2</v>
+        <v>-2.0639092188484569E-2</v>
       </c>
       <c r="G16" s="10">
         <f>D16/D$16</f>
@@ -32607,27 +32600,27 @@
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19:G23" si="22">B11-B3</f>
-        <v>-868332.21099887788</v>
+        <v>-1194258.4916722756</v>
       </c>
       <c r="C19" s="2">
         <f t="shared" si="22"/>
-        <v>868332.21099887788</v>
+        <v>840115.93611672334</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>-354142.55555555224</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="22"/>
-        <v>-1736664.4219977558</v>
+        <v>-2034374.4277889989</v>
       </c>
       <c r="F19" s="10">
         <f t="shared" si="22"/>
-        <v>-0.10262626262626262</v>
+        <v>-0.10262626262626273</v>
       </c>
       <c r="G19" s="10">
         <f t="shared" si="22"/>
-        <v>1.1111111111111183E-3</v>
+        <v>1.1111111111111321E-3</v>
       </c>
       <c r="I19" t="s">
         <v>16</v>
@@ -32672,19 +32665,19 @@
       </c>
       <c r="B20" s="2">
         <f t="shared" si="22"/>
-        <v>-777121.7327918373</v>
+        <v>-979686.77361241356</v>
       </c>
       <c r="C20" s="2">
         <f t="shared" si="22"/>
-        <v>2315505.5711756758</v>
+        <v>2196326.8039154448</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="22"/>
-        <v>1538383.8383838385</v>
+        <v>1216640.0303030312</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="22"/>
-        <v>-3092627.3039675131</v>
+        <v>-3176013.5775278583</v>
       </c>
       <c r="F20" s="10">
         <f t="shared" si="22"/>
@@ -32696,51 +32689,51 @@
       </c>
       <c r="I20" s="2">
         <f>G3*$D$8*F19</f>
-        <v>-1736664.4219977553</v>
+        <v>-1773239.0080359166</v>
       </c>
       <c r="J20" s="3">
         <f>$D$8*F3*G19</f>
-        <v>143582.49158249251</v>
+        <v>146606.37468013747</v>
       </c>
       <c r="K20" s="3">
         <f>F3*G3*$D$24</f>
-        <v>-142146.66666666669</v>
+        <v>-439645.26013333403</v>
       </c>
       <c r="L20" s="3">
         <f>SUM(I20:K20)</f>
-        <v>-1735228.5970819294</v>
+        <v>-2066277.8934891131</v>
       </c>
       <c r="M20" s="3">
         <f>L20-E19</f>
-        <v>1435.8249158263206</v>
+        <v>-31903.465700114146</v>
       </c>
       <c r="N20" s="5">
         <f>M20/E19</f>
-        <v>-8.2677165354411576E-4</v>
+        <v>1.5682199532358214E-2</v>
       </c>
       <c r="P20" s="2">
         <f>G27*$D$8*F43</f>
-        <v>1736664.4219977553</v>
+        <v>1773239.0080359166</v>
       </c>
       <c r="Q20" s="3">
         <f>$C$8*F27*G43</f>
-        <v>-68336.739052115445</v>
+        <v>-69775.927827086271</v>
       </c>
       <c r="R20" s="3">
         <f>F27*G27*$C$24</f>
-        <v>-416144.85264276154</v>
+        <v>-274617.33507244877</v>
       </c>
       <c r="S20" s="3">
         <f>SUM(P20:R20)</f>
-        <v>1252182.8303028783</v>
+        <v>1428845.7451363816</v>
       </c>
       <c r="T20" s="3">
         <f>S20+E19</f>
-        <v>-484481.59169487748</v>
+        <v>-605528.68265261734</v>
       </c>
       <c r="U20" s="5">
         <f>T20/-E19</f>
-        <v>-0.2789724863123289</v>
+        <v>-0.29764859132186333</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
@@ -32749,75 +32742,75 @@
       </c>
       <c r="B21" s="2">
         <f t="shared" si="22"/>
-        <v>-1635544.9229133436</v>
+        <v>-1725907.1526847421</v>
       </c>
       <c r="C21" s="2">
         <f t="shared" si="22"/>
-        <v>97161.084529505111</v>
+        <v>58540.233492822852</v>
       </c>
       <c r="D21" s="2">
         <f t="shared" si="22"/>
-        <v>-1538383.8383838385</v>
+        <v>-1667366.9191919193</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="22"/>
-        <v>-1732706.0074428488</v>
+        <v>-1784447.386177565</v>
       </c>
       <c r="F21" s="10">
         <f t="shared" si="22"/>
-        <v>-0.24210526315789457</v>
+        <v>-0.24210526315789471</v>
       </c>
       <c r="G21" s="10">
         <f t="shared" si="22"/>
-        <v>-9.6969696969696935E-3</v>
+        <v>-9.6969696969697004E-3</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" ref="I21:I24" si="23">G4*$D$8*F20</f>
-        <v>-3171925.43996668</v>
+        <v>-3238726.9811517261</v>
       </c>
       <c r="J21" s="3">
         <f t="shared" ref="J21:J24" si="24">$D$8*F4*G20</f>
-        <v>440545.1999953721</v>
+        <v>449823.19182662875</v>
       </c>
       <c r="K21" s="3">
         <f t="shared" ref="K21:K24" si="25">F4*G4*$D$24</f>
-        <v>-39649.06799958348</v>
+        <v>-122630.55633656181</v>
       </c>
       <c r="L21" s="3">
         <f t="shared" ref="L21:L24" si="26">SUM(I21:K21)</f>
-        <v>-2771029.3079708917</v>
+        <v>-2911534.3456616593</v>
       </c>
       <c r="M21" s="3">
         <f t="shared" ref="M21:M24" si="27">L21-E20</f>
-        <v>321597.99599662144</v>
+        <v>264479.23186619906</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" ref="N21:N24" si="28">M21/E20</f>
-        <v>-0.10398860398860389</v>
+        <v>-8.3273961338686753E-2</v>
       </c>
       <c r="P21" s="2">
         <f t="shared" ref="P21:P24" si="29">G28*$D$8*F44</f>
-        <v>3171925.43996668</v>
+        <v>3238726.9811517261</v>
       </c>
       <c r="Q21" s="3">
         <f t="shared" ref="Q21:Q24" si="30">$C$8*F28*G44</f>
-        <v>-209673.35251630782</v>
+        <v>-214089.12563538604</v>
       </c>
       <c r="R21" s="3">
         <f t="shared" ref="R21:R24" si="31">F28*G28*$C$24</f>
-        <v>-116075.57142934175</v>
+        <v>-76599.203115223208</v>
       </c>
       <c r="S21" s="3">
         <f t="shared" ref="S21:S24" si="32">SUM(P21:R21)</f>
-        <v>2846176.5160210305</v>
+        <v>2948038.6524011167</v>
       </c>
       <c r="T21" s="3">
         <f t="shared" ref="T21:T24" si="33">S21+E20</f>
-        <v>-246450.78794648265</v>
+        <v>-227974.92512674164</v>
       </c>
       <c r="U21" s="5">
         <f t="shared" ref="U21:U24" si="34">T21/-E20</f>
-        <v>-7.9689779505701316E-2</v>
+        <v>-7.1780211123717075E-2</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
@@ -32826,75 +32819,75 @@
       </c>
       <c r="B22" s="2">
         <f t="shared" si="22"/>
-        <v>176273.14814814832</v>
+        <v>138735.94560185215</v>
       </c>
       <c r="C22" s="2">
         <f t="shared" si="22"/>
-        <v>1362110.6902356902</v>
+        <v>1335462.3069234004</v>
       </c>
       <c r="D22" s="2">
         <f t="shared" si="22"/>
-        <v>1538383.8383838385</v>
+        <v>1474198.2525252528</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="22"/>
-        <v>-1185837.5420875419</v>
+        <v>-1196726.3613215482</v>
       </c>
       <c r="F22" s="10">
         <f t="shared" si="22"/>
-        <v>-0.31249999999999989</v>
+        <v>-0.31249999999999978</v>
       </c>
       <c r="G22" s="10">
         <f t="shared" si="22"/>
-        <v>1.0303030303030307E-2</v>
+        <v>1.0303030303030303E-2</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" si="23"/>
-        <v>-1489803.2961190848</v>
+        <v>-1521178.9252525254</v>
       </c>
       <c r="J22" s="3">
         <f t="shared" si="24"/>
-        <v>-596706.45852464007</v>
+        <v>-609273.2454239364</v>
       </c>
       <c r="K22" s="3">
         <f t="shared" si="25"/>
-        <v>-24614.141414141417</v>
+        <v>-76129.049373737493</v>
       </c>
       <c r="L22" s="3">
         <f t="shared" si="26"/>
-        <v>-2111123.896057866</v>
+        <v>-2206581.2200501994</v>
       </c>
       <c r="M22" s="3">
         <f t="shared" si="27"/>
-        <v>-378417.88861501729</v>
+        <v>-422133.83387263445</v>
       </c>
       <c r="N22" s="5">
         <f t="shared" si="28"/>
-        <v>0.21839705465873671</v>
+        <v>0.23656277968322748</v>
       </c>
       <c r="P22" s="2">
         <f t="shared" si="29"/>
-        <v>1489803.2961190848</v>
+        <v>1521178.9252525254</v>
       </c>
       <c r="Q22" s="3">
         <f t="shared" si="30"/>
-        <v>283996.8376191791</v>
+        <v>289977.88187879458</v>
       </c>
       <c r="R22" s="3">
         <f t="shared" si="31"/>
-        <v>-72059.714743335338</v>
+        <v>-47552.785293930516</v>
       </c>
       <c r="S22" s="3">
         <f t="shared" si="32"/>
-        <v>1701740.4189949287</v>
+        <v>1763604.0218373896</v>
       </c>
       <c r="T22" s="3">
         <f t="shared" si="33"/>
-        <v>-30965.588447920047</v>
+        <v>-20843.364340175409</v>
       </c>
       <c r="U22" s="5">
         <f t="shared" si="34"/>
-        <v>-1.7871230500100525E-2</v>
+        <v>-1.1680570972071994E-2</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
@@ -32903,75 +32896,75 @@
       </c>
       <c r="B23" s="2">
         <f t="shared" si="22"/>
-        <v>-2937390.2912863865</v>
+        <v>-3968998.1943616718</v>
       </c>
       <c r="C23" s="2">
         <f t="shared" si="22"/>
-        <v>-139377.38548129052</v>
+        <v>-1458396.1995777339</v>
       </c>
       <c r="D23" s="2">
         <f t="shared" si="22"/>
-        <v>-3076767.6767676771</v>
+        <v>-5427394.3939394057</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="22"/>
-        <v>-2798012.905805096</v>
+        <v>-2510601.9947839379</v>
       </c>
       <c r="F23" s="10">
         <f t="shared" si="22"/>
-        <v>-2.9066171923314621E-2</v>
+        <v>-2.9066171923314649E-2</v>
       </c>
       <c r="G23" s="10">
         <f t="shared" si="22"/>
-        <v>-1.2828282828282744E-2</v>
+        <v>-1.2828282828282855E-2</v>
       </c>
       <c r="I23" s="2">
         <f t="shared" si="23"/>
-        <v>-961489.89898989873</v>
+        <v>-981739.1161616157</v>
       </c>
       <c r="J23" s="3">
         <f t="shared" si="24"/>
-        <v>264166.92174267932</v>
+        <v>269730.34302622156</v>
       </c>
       <c r="K23" s="3">
         <f t="shared" si="25"/>
-        <v>-5127.9461279461257</v>
+        <v>-15860.218619528629</v>
       </c>
       <c r="L23" s="3">
         <f t="shared" si="26"/>
-        <v>-702450.92337516556</v>
+        <v>-727868.99175492267</v>
       </c>
       <c r="M23" s="3">
         <f t="shared" si="27"/>
-        <v>483386.61871237634</v>
+        <v>468857.36956662557</v>
       </c>
       <c r="N23" s="5">
         <f t="shared" si="28"/>
-        <v>-0.40763308763308775</v>
+        <v>-0.39178327203293584</v>
       </c>
       <c r="P23" s="2">
         <f t="shared" si="29"/>
-        <v>961489.89898989873</v>
+        <v>981739.1161616157</v>
       </c>
       <c r="Q23" s="3">
         <f t="shared" si="30"/>
-        <v>-125727.76665432412</v>
+        <v>-128375.62479009123</v>
       </c>
       <c r="R23" s="3">
         <f t="shared" si="31"/>
-        <v>-15012.440571528186</v>
+        <v>-9906.830269568849</v>
       </c>
       <c r="S23" s="3">
         <f t="shared" si="32"/>
-        <v>820749.69176404644</v>
+        <v>843456.66110195569</v>
       </c>
       <c r="T23" s="3">
         <f t="shared" si="33"/>
-        <v>-365087.85032349546</v>
+        <v>-353269.70021959255</v>
       </c>
       <c r="U23" s="5">
         <f t="shared" si="34"/>
-        <v>-0.30787341213771729</v>
+        <v>-0.29519672302486583</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
@@ -32980,23 +32973,23 @@
       </c>
       <c r="B24" s="3">
         <f>SUM(B19:B23)</f>
-        <v>-6042116.0098422971</v>
+        <v>-7730114.6667292509</v>
       </c>
       <c r="C24" s="3">
         <f>SUM(C19:C23)</f>
-        <v>4503732.1714584585</v>
+        <v>2972049.0808706572</v>
       </c>
       <c r="D24" s="3">
         <f>SUM(D19:D23)</f>
-        <v>-1538383.8383838385</v>
+        <v>-4758065.5858585928</v>
       </c>
       <c r="E24" s="3">
         <f>SUM(E19:E23)</f>
-        <v>-10545848.181300756</v>
+        <v>-10702163.747599907</v>
       </c>
       <c r="F24" s="10">
         <f>F16-F8</f>
-        <v>-6.8757866296065701E-2</v>
+        <v>-6.8757866296065714E-2</v>
       </c>
       <c r="G24" s="10">
         <f>G16-G8</f>
@@ -33004,109 +32997,109 @@
       </c>
       <c r="I24" s="2">
         <f t="shared" si="23"/>
-        <v>-3264189.8265274707</v>
+        <v>-3332934.4787141518</v>
       </c>
       <c r="J24" s="3">
         <f t="shared" si="24"/>
-        <v>241650.89359894415</v>
+        <v>246740.12171186265</v>
       </c>
       <c r="K24" s="3">
         <f t="shared" si="25"/>
-        <v>137512.67779839216</v>
+        <v>425312.80134817655</v>
       </c>
       <c r="L24" s="3">
         <f t="shared" si="26"/>
-        <v>-2885026.2551301345</v>
+        <v>-2660881.5556541122</v>
       </c>
       <c r="M24" s="3">
         <f t="shared" si="27"/>
-        <v>-87013.349325038493</v>
+        <v>-150279.56087017432</v>
       </c>
       <c r="N24" s="5">
         <f t="shared" si="28"/>
-        <v>3.1098265895954259E-2</v>
+        <v>5.9857978756647709E-2</v>
       </c>
       <c r="P24" s="2">
         <f t="shared" si="29"/>
-        <v>3264189.8265274707</v>
+        <v>3332934.4787141518</v>
       </c>
       <c r="Q24" s="3">
         <f t="shared" si="30"/>
-        <v>-115011.47441848071</v>
+        <v>-117433.64476596625</v>
       </c>
       <c r="R24" s="3">
         <f t="shared" si="31"/>
-        <v>402578.50838751142</v>
+        <v>265664.79539211199</v>
       </c>
       <c r="S24" s="3">
         <f t="shared" si="32"/>
-        <v>3551756.8604965014</v>
+        <v>3481165.6293402975</v>
       </c>
       <c r="T24" s="3">
         <f t="shared" si="33"/>
-        <v>753743.95469140541</v>
+        <v>970563.63455635961</v>
       </c>
       <c r="U24" s="5">
         <f t="shared" si="34"/>
-        <v>0.26938544605266007</v>
+        <v>0.38658602063282682</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I25" s="3">
         <f>SUM(I20:I24)</f>
-        <v>-10624072.883600891</v>
+        <v>-10847818.509315936</v>
       </c>
       <c r="J25" s="3">
         <f>SUM(J20:J24)</f>
-        <v>493239.04839484801</v>
+        <v>503626.78582091408</v>
       </c>
       <c r="K25" s="3">
         <f>SUM(K20:K24)</f>
-        <v>-74025.144409945584</v>
+        <v>-228952.28311498545</v>
       </c>
       <c r="L25" s="3">
         <f t="shared" ref="L25" si="35">SUM(I25:K25)</f>
-        <v>-10204858.979615988</v>
+        <v>-10573144.006610006</v>
       </c>
       <c r="M25" s="3">
         <f>L25-E24</f>
-        <v>340989.20168476738</v>
+        <v>129019.74098990113</v>
       </c>
       <c r="N25" s="5">
         <f>M25/E24</f>
-        <v>-3.2333975970694165E-2</v>
+        <v>-1.2055481866350195E-2</v>
       </c>
       <c r="P25" s="3">
         <f>SUM(P20:P24)</f>
-        <v>10624072.883600891</v>
+        <v>10847818.509315936</v>
       </c>
       <c r="Q25" s="3">
         <f>SUM(Q20:Q24)</f>
-        <v>-234752.495022049</v>
+        <v>-239696.44113973517</v>
       </c>
       <c r="R25" s="3">
         <f>SUM(R20:R24)</f>
-        <v>-216714.07099945546</v>
+        <v>-143011.35835905932</v>
       </c>
       <c r="S25" s="3">
         <f t="shared" ref="S25" si="36">SUM(P25:R25)</f>
-        <v>10172606.317579387</v>
+        <v>10465110.709817141</v>
       </c>
       <c r="T25" s="3">
         <f>S25+E24</f>
-        <v>-373241.86372136883</v>
+        <v>-237053.03778276592</v>
       </c>
       <c r="U25" s="5">
         <f>T25/-E24</f>
-        <v>-3.5392303900522497E-2</v>
+        <v>-2.2150010350563736E-2</v>
       </c>
       <c r="W25" s="2" cm="1">
         <f t="array" ref="W25">SUM(ABS(M20:M24))</f>
-        <v>1271851.6775648799</v>
+        <v>1337653.4618757474</v>
       </c>
       <c r="X25" s="2" cm="1">
         <f t="array" ref="X25">SUM(ABS(T20:T24))</f>
-        <v>1880729.773104181</v>
+        <v>2178180.3068954865</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
@@ -33138,7 +33131,7 @@
       </c>
       <c r="F27" s="5">
         <f>-E3/D3</f>
-        <v>-0.84</v>
+        <v>-0.84000000000000008</v>
       </c>
       <c r="G27" s="5">
         <f>G3</f>
@@ -33173,11 +33166,11 @@
       <c r="E28" s="10"/>
       <c r="F28" s="5">
         <f>-E4/D4</f>
-        <v>-0.25773195876288668</v>
+        <v>-0.25773195876288685</v>
       </c>
       <c r="G28" s="5">
         <f>G4</f>
-        <v>0.1</v>
+        <v>0.10000000000000002</v>
       </c>
       <c r="I28" t="s">
         <v>16</v>
@@ -33227,89 +33220,89 @@
       </c>
       <c r="F29" s="5">
         <f t="shared" ref="F29:F31" si="37">-E5/D5</f>
-        <v>-0.39999999999999997</v>
+        <v>-0.39999999999999991</v>
       </c>
       <c r="G29" s="5">
         <f t="shared" ref="G29:G31" si="38">G5</f>
-        <v>0.04</v>
+        <v>4.0000000000000008E-2</v>
       </c>
       <c r="I29" s="2">
         <f>G3*$D$8*F19</f>
-        <v>-1736664.4219977553</v>
+        <v>-1773239.0080359166</v>
       </c>
       <c r="J29" s="3">
         <f>$D$8*F11*G19</f>
-        <v>126040.42671382822</v>
+        <v>128694.86954846121</v>
       </c>
       <c r="K29" s="3">
         <f>F11*G11*$D$24</f>
-        <v>-126040.4267138274</v>
+        <v>-389830.28930154582</v>
       </c>
       <c r="L29" s="3">
         <f>SUM(I29:K29)</f>
-        <v>-1736664.4219977544</v>
+        <v>-2034374.4277890013</v>
       </c>
       <c r="M29" s="3">
         <f>L29-E19</f>
-        <v>0</v>
+        <v>-2.3283064365386963E-9</v>
       </c>
       <c r="N29" s="1">
         <f>M29/E19</f>
-        <v>0</v>
+        <v>1.1444827484727818E-15</v>
       </c>
       <c r="P29" s="2">
         <f>G27*$D$8*F43</f>
-        <v>1736664.4219977553</v>
+        <v>1773239.0080359166</v>
       </c>
       <c r="Q29" s="3">
         <f>$D$8*F35*G43</f>
-        <v>-126040.42671382822</v>
+        <v>-128694.86954846121</v>
       </c>
       <c r="R29" s="3">
         <f>F35*G35*$D$24</f>
-        <v>126040.4267138274</v>
+        <v>389830.28930154582</v>
       </c>
       <c r="S29" s="3">
         <f>SUM(P29:R29)</f>
-        <v>1736664.4219977544</v>
+        <v>2034374.4277890013</v>
       </c>
       <c r="T29" s="3">
         <f>S29+E19</f>
-        <v>0</v>
+        <v>2.3283064365386963E-9</v>
       </c>
       <c r="U29" s="1">
         <f>T29/-E19</f>
-        <v>0</v>
+        <v>1.1444827484727818E-15</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D30" s="3">
         <f>(C29-D29)*D16</f>
-        <v>-1736664.4219977537</v>
+        <v>-1736894.6811223328</v>
       </c>
       <c r="F30" s="5">
         <f t="shared" si="37"/>
-        <v>-0.16666666666666657</v>
+        <v>-0.16666666666666649</v>
       </c>
       <c r="G30" s="5">
         <f t="shared" si="38"/>
-        <v>0.02</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="I30" s="2">
         <f t="shared" ref="I30:I33" si="39">G4*$D$8*F20</f>
-        <v>-3171925.43996668</v>
+        <v>-3238726.9811517261</v>
       </c>
       <c r="J30" s="3">
         <f t="shared" ref="J30:J33" si="40">$D$8*F12*G20</f>
-        <v>88109.039999074274</v>
+        <v>89964.638365325853</v>
       </c>
       <c r="K30" s="3">
         <f t="shared" ref="K30:K33" si="41">F12*G12*$D$24</f>
-        <v>-8810.9039999074266</v>
+        <v>-27251.234741458207</v>
       </c>
       <c r="L30" s="3">
         <f t="shared" ref="L30:L33" si="42">SUM(I30:K30)</f>
-        <v>-3092627.3039675131</v>
+        <v>-3176013.5775278583</v>
       </c>
       <c r="M30" s="3">
         <f t="shared" ref="M30:M33" si="43">L30-E20</f>
@@ -33321,19 +33314,19 @@
       </c>
       <c r="P30" s="2">
         <f t="shared" ref="P30:P33" si="45">G28*$D$8*F44</f>
-        <v>3171925.43996668</v>
+        <v>3238726.9811517261</v>
       </c>
       <c r="Q30" s="3">
         <f t="shared" ref="Q30:Q33" si="46">$D$8*F36*G44</f>
-        <v>-88109.039999074274</v>
+        <v>-89964.638365325853</v>
       </c>
       <c r="R30" s="3">
         <f t="shared" ref="R30:R33" si="47">F36*G36*$D$24</f>
-        <v>8810.9039999074266</v>
+        <v>27251.234741458207</v>
       </c>
       <c r="S30" s="3">
         <f t="shared" ref="S30:S33" si="48">SUM(P30:R30)</f>
-        <v>3092627.3039675131</v>
+        <v>3176013.5775278583</v>
       </c>
       <c r="T30" s="3">
         <f t="shared" ref="T30:T33" si="49">S30+E20</f>
@@ -33351,23 +33344,23 @@
       </c>
       <c r="G31" s="5">
         <f t="shared" si="38"/>
-        <v>0.72999999999999987</v>
+        <v>0.73</v>
       </c>
       <c r="I31" s="2">
         <f t="shared" si="39"/>
-        <v>-1489803.2961190848</v>
+        <v>-1521178.9252525254</v>
       </c>
       <c r="J31" s="3">
         <f t="shared" si="40"/>
-        <v>-235542.02310183184</v>
+        <v>-240502.5968778696</v>
       </c>
       <c r="K31" s="3">
         <f t="shared" si="41"/>
-        <v>-7360.6882219322497</v>
+        <v>-22765.864047170297</v>
       </c>
       <c r="L31" s="3">
         <f t="shared" si="42"/>
-        <v>-1732706.0074428488</v>
+        <v>-1784447.3861775654</v>
       </c>
       <c r="M31" s="3">
         <f t="shared" si="43"/>
@@ -33379,19 +33372,19 @@
       </c>
       <c r="P31" s="2">
         <f t="shared" si="45"/>
-        <v>1489803.2961190848</v>
+        <v>1521178.9252525254</v>
       </c>
       <c r="Q31" s="3">
         <f t="shared" si="46"/>
-        <v>235542.02310183184</v>
+        <v>240502.5968778696</v>
       </c>
       <c r="R31" s="3">
         <f t="shared" si="47"/>
-        <v>7360.6882219322497</v>
+        <v>22765.864047170297</v>
       </c>
       <c r="S31" s="3">
         <f t="shared" si="48"/>
-        <v>1732706.0074428488</v>
+        <v>1784447.3861775654</v>
       </c>
       <c r="T31" s="3">
         <f t="shared" si="49"/>
@@ -33411,7 +33404,7 @@
       </c>
       <c r="F32" s="5">
         <f>-E8/D8</f>
-        <v>-4.8118774107581114E-2</v>
+        <v>-4.8118774107581148E-2</v>
       </c>
       <c r="G32" s="5">
         <f>G8</f>
@@ -33419,19 +33412,19 @@
       </c>
       <c r="I32" s="2">
         <f t="shared" si="39"/>
-        <v>-961489.89898989873</v>
+        <v>-981739.1161616157</v>
       </c>
       <c r="J32" s="3">
         <f t="shared" si="40"/>
-        <v>-231146.05652484455</v>
+        <v>-236014.05014794401</v>
       </c>
       <c r="K32" s="3">
         <f t="shared" si="41"/>
-        <v>6798.413427201308</v>
+        <v>21026.804988011452</v>
       </c>
       <c r="L32" s="3">
         <f t="shared" si="42"/>
-        <v>-1185837.5420875419</v>
+        <v>-1196726.3613215482</v>
       </c>
       <c r="M32" s="3">
         <f t="shared" si="43"/>
@@ -33443,19 +33436,19 @@
       </c>
       <c r="P32" s="2">
         <f t="shared" si="45"/>
-        <v>961489.89898989873</v>
+        <v>981739.1161616157</v>
       </c>
       <c r="Q32" s="3">
         <f t="shared" si="46"/>
-        <v>231146.05652484455</v>
+        <v>236014.05014794401</v>
       </c>
       <c r="R32" s="3">
         <f t="shared" si="47"/>
-        <v>-6798.413427201308</v>
+        <v>-21026.804988011452</v>
       </c>
       <c r="S32" s="3">
         <f t="shared" si="48"/>
-        <v>1185837.5420875419</v>
+        <v>1196726.3613215482</v>
       </c>
       <c r="T32" s="3">
         <f t="shared" si="49"/>
@@ -33477,19 +33470,19 @@
       </c>
       <c r="I33" s="2">
         <f t="shared" si="39"/>
-        <v>-3264189.8265274707</v>
+        <v>-3332934.4787141518</v>
       </c>
       <c r="J33" s="3">
         <f t="shared" si="40"/>
-        <v>299012.46935222851</v>
+        <v>305309.74656265799</v>
       </c>
       <c r="K33" s="3">
         <f t="shared" si="41"/>
-        <v>167164.45137014458</v>
+        <v>517022.73736755428</v>
       </c>
       <c r="L33" s="3">
         <f t="shared" si="42"/>
-        <v>-2798012.9058050974</v>
+        <v>-2510601.9947839398</v>
       </c>
       <c r="M33" s="3">
         <f t="shared" si="43"/>
@@ -33501,19 +33494,19 @@
       </c>
       <c r="P33" s="2">
         <f t="shared" si="45"/>
-        <v>3264189.8265274707</v>
+        <v>3332934.4787141518</v>
       </c>
       <c r="Q33" s="3">
         <f t="shared" si="46"/>
-        <v>-299012.46935222851</v>
+        <v>-305309.74656265799</v>
       </c>
       <c r="R33" s="3">
         <f t="shared" si="47"/>
-        <v>-167164.45137014458</v>
+        <v>-517022.73736755428</v>
       </c>
       <c r="S33" s="3">
         <f t="shared" si="48"/>
-        <v>2798012.9058050974</v>
+        <v>2510601.9947839398</v>
       </c>
       <c r="T33" s="3">
         <f t="shared" si="49"/>
@@ -33541,19 +33534,19 @@
       </c>
       <c r="I34" s="3">
         <f>SUM(I29:I33)</f>
-        <v>-10624072.883600891</v>
+        <v>-10847818.509315936</v>
       </c>
       <c r="J34" s="3">
         <f>SUM(J29:J33)</f>
-        <v>46473.85643845459</v>
+        <v>47452.607450631447</v>
       </c>
       <c r="K34" s="3">
         <f>SUM(K29:K33)</f>
-        <v>31750.845861678827</v>
+        <v>98202.154265391408</v>
       </c>
       <c r="L34" s="3">
         <f t="shared" ref="L34" si="51">SUM(I34:K34)</f>
-        <v>-10545848.181300757</v>
+        <v>-10702163.747599913</v>
       </c>
       <c r="M34" s="3">
         <f>L34-E24</f>
@@ -33565,19 +33558,19 @@
       </c>
       <c r="P34" s="3">
         <f>SUM(P29:P33)</f>
-        <v>10624072.883600891</v>
+        <v>10847818.509315936</v>
       </c>
       <c r="Q34" s="3">
         <f>SUM(Q29:Q33)</f>
-        <v>-46473.85643845459</v>
+        <v>-47452.607450631447</v>
       </c>
       <c r="R34" s="3">
         <f>SUM(R29:R33)</f>
-        <v>-31750.845861678827</v>
+        <v>-98202.154265391408</v>
       </c>
       <c r="S34" s="3">
         <f t="shared" ref="S34" si="52">SUM(P34:R34)</f>
-        <v>10545848.181300757</v>
+        <v>10702163.747599913</v>
       </c>
       <c r="T34" s="3">
         <f>S34+E24</f>
@@ -33603,21 +33596,21 @@
       </c>
       <c r="G35" s="5">
         <f>G11</f>
-        <v>0.11111111111111112</v>
+        <v>0.11111111111111113</v>
       </c>
     </row>
     <row r="36" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D36" s="3">
         <f>(C35-D35)*D16</f>
-        <v>-3092627.3039675127</v>
+        <v>-3093037.3461418333</v>
       </c>
       <c r="F36" s="5">
         <f t="shared" ref="F36:F39" si="53">-E12/D12</f>
-        <v>-5.1546391752577254E-2</v>
+        <v>-5.1546391752577421E-2</v>
       </c>
       <c r="G36" s="5">
         <f t="shared" ref="G36:G39" si="54">G12</f>
-        <v>0.11111111111111112</v>
+        <v>0.11111111111111113</v>
       </c>
       <c r="I36" s="50" t="s">
         <v>39</v>
@@ -33639,7 +33632,7 @@
     <row r="37" spans="3:21" x14ac:dyDescent="0.25">
       <c r="F37" s="5">
         <f t="shared" si="53"/>
-        <v>-0.15789473684210539</v>
+        <v>-0.1578947368421052</v>
       </c>
       <c r="G37" s="5">
         <f t="shared" si="54"/>
@@ -33651,15 +33644,15 @@
       </c>
       <c r="J37" s="3">
         <f t="shared" si="55"/>
-        <v>17542.064868664296</v>
+        <v>17911.505131676255</v>
       </c>
       <c r="K37" s="3">
         <f t="shared" si="55"/>
-        <v>-16106.239952839285</v>
+        <v>-49814.970831788203</v>
       </c>
       <c r="L37" s="3">
         <f t="shared" si="55"/>
-        <v>1435.8249158249237</v>
+        <v>-31903.465700111818</v>
       </c>
       <c r="P37" s="3">
         <f t="shared" ref="P37:S42" si="56">P20-P29</f>
@@ -33667,15 +33660,15 @@
       </c>
       <c r="Q37" s="3">
         <f t="shared" si="56"/>
-        <v>57703.687661712771</v>
+        <v>58918.94172137494</v>
       </c>
       <c r="R37" s="3">
         <f t="shared" si="56"/>
-        <v>-542185.27935658896</v>
+        <v>-664447.62437399453</v>
       </c>
       <c r="S37" s="3">
         <f t="shared" si="56"/>
-        <v>-484481.59169487609</v>
+        <v>-605528.68265261967</v>
       </c>
     </row>
     <row r="38" spans="3:21" x14ac:dyDescent="0.25">
@@ -33687,7 +33680,7 @@
       </c>
       <c r="F38" s="5">
         <f t="shared" si="53"/>
-        <v>0.14583333333333334</v>
+        <v>0.14583333333333329</v>
       </c>
       <c r="G38" s="5">
         <f t="shared" si="54"/>
@@ -33699,15 +33692,15 @@
       </c>
       <c r="J38" s="3">
         <f t="shared" si="55"/>
-        <v>352436.15999629779</v>
+        <v>359858.55346130289</v>
       </c>
       <c r="K38" s="3">
         <f t="shared" si="55"/>
-        <v>-30838.163999676053</v>
+        <v>-95379.321595103611</v>
       </c>
       <c r="L38" s="3">
         <f t="shared" si="55"/>
-        <v>321597.99599662144</v>
+        <v>264479.23186619906</v>
       </c>
       <c r="P38" s="3">
         <f t="shared" si="56"/>
@@ -33715,15 +33708,15 @@
       </c>
       <c r="Q38" s="3">
         <f t="shared" si="56"/>
-        <v>-121564.31251723354</v>
+        <v>-124124.48727006018</v>
       </c>
       <c r="R38" s="3">
         <f t="shared" si="56"/>
-        <v>-124886.47542924919</v>
+        <v>-103850.43785668141</v>
       </c>
       <c r="S38" s="3">
         <f t="shared" si="56"/>
-        <v>-246450.78794648265</v>
+        <v>-227974.92512674164</v>
       </c>
     </row>
     <row r="39" spans="3:21" x14ac:dyDescent="0.25">
@@ -33737,7 +33730,7 @@
       </c>
       <c r="F39" s="5">
         <f t="shared" si="53"/>
-        <v>0.15151515151515144</v>
+        <v>0.15151515151515146</v>
       </c>
       <c r="G39" s="5">
         <f t="shared" si="54"/>
@@ -33749,15 +33742,15 @@
       </c>
       <c r="J39" s="3">
         <f t="shared" si="55"/>
-        <v>-361164.43542280822</v>
+        <v>-368770.64854606683</v>
       </c>
       <c r="K39" s="3">
         <f t="shared" si="55"/>
-        <v>-17253.453192209166</v>
+        <v>-53363.185326567196</v>
       </c>
       <c r="L39" s="3">
         <f t="shared" si="55"/>
-        <v>-378417.88861501729</v>
+        <v>-422133.83387263399</v>
       </c>
       <c r="P39" s="3">
         <f t="shared" si="56"/>
@@ -33765,15 +33758,15 @@
       </c>
       <c r="Q39" s="3">
         <f t="shared" si="56"/>
-        <v>48454.814517347259</v>
+        <v>49475.285000924981</v>
       </c>
       <c r="R39" s="3">
         <f t="shared" si="56"/>
-        <v>-79420.402965267582</v>
+        <v>-70318.649341100812</v>
       </c>
       <c r="S39" s="3">
         <f t="shared" si="56"/>
-        <v>-30965.588447920047</v>
+        <v>-20843.364340175875</v>
       </c>
     </row>
     <row r="40" spans="3:21" x14ac:dyDescent="0.25">
@@ -33787,7 +33780,7 @@
       </c>
       <c r="F40" s="5">
         <f>-E16/D16</f>
-        <v>2.0639092188484587E-2</v>
+        <v>2.0639092188484569E-2</v>
       </c>
       <c r="G40" s="5">
         <f>G16</f>
@@ -33799,15 +33792,15 @@
       </c>
       <c r="J40" s="3">
         <f t="shared" si="55"/>
-        <v>495312.97826752387</v>
+        <v>505744.39317416557</v>
       </c>
       <c r="K40" s="3">
         <f t="shared" si="55"/>
-        <v>-11926.359555147434</v>
+        <v>-36887.023607540083</v>
       </c>
       <c r="L40" s="3">
         <f t="shared" si="55"/>
-        <v>483386.61871237634</v>
+        <v>468857.36956662557</v>
       </c>
       <c r="P40" s="3">
         <f t="shared" si="56"/>
@@ -33815,15 +33808,15 @@
       </c>
       <c r="Q40" s="3">
         <f t="shared" si="56"/>
-        <v>-356873.82317916868</v>
+        <v>-364389.67493803526</v>
       </c>
       <c r="R40" s="3">
         <f t="shared" si="56"/>
-        <v>-8214.0271443268794</v>
+        <v>11119.974718442603</v>
       </c>
       <c r="S40" s="3">
         <f t="shared" si="56"/>
-        <v>-365087.85032349546</v>
+        <v>-353269.70021959255</v>
       </c>
     </row>
     <row r="41" spans="3:21" x14ac:dyDescent="0.25">
@@ -33841,15 +33834,15 @@
       </c>
       <c r="J41" s="3">
         <f t="shared" si="55"/>
-        <v>-57361.575753284356</v>
+        <v>-58569.624850795342</v>
       </c>
       <c r="K41" s="3">
         <f t="shared" si="55"/>
-        <v>-29651.773571752419</v>
+        <v>-91709.936019377725</v>
       </c>
       <c r="L41" s="3">
         <f t="shared" si="55"/>
-        <v>-87013.349325037096</v>
+        <v>-150279.56087017246</v>
       </c>
       <c r="P41" s="3">
         <f t="shared" si="56"/>
@@ -33857,21 +33850,21 @@
       </c>
       <c r="Q41" s="3">
         <f t="shared" si="56"/>
-        <v>184000.9949337478</v>
+        <v>187876.10179669174</v>
       </c>
       <c r="R41" s="3">
         <f t="shared" si="56"/>
-        <v>569742.95975765598</v>
+        <v>782687.53275966621</v>
       </c>
       <c r="S41" s="3">
         <f t="shared" si="56"/>
-        <v>753743.95469140401</v>
+        <v>970563.63455635775</v>
       </c>
     </row>
     <row r="42" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D42" s="3">
         <f>(C41-D41)*D16</f>
-        <v>-1672756.9573283733</v>
+        <v>-1672978.7431539763</v>
       </c>
       <c r="F42" t="s">
         <v>21</v>
@@ -33885,15 +33878,15 @@
       </c>
       <c r="J42" s="3">
         <f t="shared" si="55"/>
-        <v>446765.19195639342</v>
+        <v>456174.17837028264</v>
       </c>
       <c r="K42" s="3">
         <f t="shared" si="55"/>
-        <v>-105775.99027162441</v>
+        <v>-327154.43738037685</v>
       </c>
       <c r="L42" s="3">
         <f t="shared" si="55"/>
-        <v>340989.20168476924</v>
+        <v>129019.74098990671</v>
       </c>
       <c r="P42" s="3">
         <f t="shared" si="56"/>
@@ -33901,25 +33894,25 @@
       </c>
       <c r="Q42" s="3">
         <f t="shared" si="56"/>
-        <v>-188278.63858359441</v>
+        <v>-192243.83368910372</v>
       </c>
       <c r="R42" s="3">
         <f t="shared" si="56"/>
-        <v>-184963.22513777664</v>
+        <v>-44809.204093667911</v>
       </c>
       <c r="S42" s="3">
         <f t="shared" si="56"/>
-        <v>-373241.8637213707</v>
+        <v>-237053.03778277151</v>
       </c>
     </row>
     <row r="43" spans="3:21" x14ac:dyDescent="0.25">
       <c r="F43" s="5">
         <f>F35-F27</f>
-        <v>0.10262626262626262</v>
+        <v>0.10262626262626273</v>
       </c>
       <c r="G43" s="5">
         <f>G35-G27</f>
-        <v>1.1111111111111183E-3</v>
+        <v>1.1111111111111321E-3</v>
       </c>
       <c r="J43" s="3"/>
     </row>
@@ -33936,37 +33929,37 @@
     <row r="45" spans="3:21" x14ac:dyDescent="0.25">
       <c r="F45" s="5">
         <f t="shared" si="57"/>
-        <v>0.24210526315789457</v>
+        <v>0.24210526315789471</v>
       </c>
       <c r="G45" s="5">
         <f t="shared" si="57"/>
-        <v>-9.6969696969696935E-3</v>
+        <v>-9.6969696969697004E-3</v>
       </c>
     </row>
     <row r="46" spans="3:21" x14ac:dyDescent="0.25">
       <c r="F46" s="5">
         <f t="shared" si="57"/>
-        <v>0.31249999999999989</v>
+        <v>0.31249999999999978</v>
       </c>
       <c r="G46" s="5">
         <f t="shared" si="57"/>
-        <v>1.0303030303030307E-2</v>
+        <v>1.0303030303030303E-2</v>
       </c>
     </row>
     <row r="47" spans="3:21" x14ac:dyDescent="0.25">
       <c r="F47" s="5">
         <f t="shared" si="57"/>
-        <v>2.9066171923314621E-2</v>
+        <v>2.9066171923314649E-2</v>
       </c>
       <c r="G47" s="5">
         <f t="shared" si="57"/>
-        <v>-1.2828282828282744E-2</v>
+        <v>-1.2828282828282855E-2</v>
       </c>
     </row>
     <row r="48" spans="3:21" x14ac:dyDescent="0.25">
       <c r="F48" s="5">
         <f>F40-F32</f>
-        <v>6.8757866296065701E-2</v>
+        <v>6.8757866296065714E-2</v>
       </c>
       <c r="G48" s="5">
         <f>G40-G32</f>

</xml_diff>